<commit_message>
Sequential A* is added
</commit_message>
<xml_diff>
--- a/Documents/Project 1 search averages.xlsx
+++ b/Documents/Project 1 search averages.xlsx
@@ -5,19 +5,20 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28379469e1c3152a/Documents/CS440 Intro to AI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/28379469e1c3152a/Documents/GitHub/IntroToAI/Documents/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="5"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Final Averages" sheetId="13" r:id="rId1"/>
-    <sheet name="Modified Euclidean distance" sheetId="1" r:id="rId2"/>
-    <sheet name="Euclidean Distance" sheetId="7" r:id="rId3"/>
-    <sheet name="Hard Cells Avoidance" sheetId="2" r:id="rId4"/>
+    <sheet name="Sequential A star" sheetId="15" r:id="rId2"/>
+    <sheet name="Modified Euclidean distance" sheetId="1" r:id="rId3"/>
+    <sheet name="Euclidean Distance" sheetId="7" r:id="rId4"/>
     <sheet name="Chebyshev Distance" sheetId="8" r:id="rId5"/>
     <sheet name="Manhattan Distance" sheetId="9" r:id="rId6"/>
+    <sheet name="Hard Cells Avoidance" sheetId="2" r:id="rId7"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -29,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="87">
   <si>
     <t>UCS nodes</t>
   </si>
@@ -281,6 +282,15 @@
   </si>
   <si>
     <t>Time in MS</t>
+  </si>
+  <si>
+    <t>1.25 weight A* cost</t>
+  </si>
+  <si>
+    <t>1.25 weight A* time</t>
+  </si>
+  <si>
+    <t>1.25 weight A* nodes</t>
   </si>
 </sst>
 </file>
@@ -900,24 +910,1258 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M52"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O1" sqref="O1:P1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1:G1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="16.85546875" customWidth="1"/>
-    <col min="5" max="6" width="12" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" t="s">
+        <v>85</v>
+      </c>
+      <c r="D1" t="s">
+        <v>84</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="B2:G2" si="0">AVERAGE(B3:B51)</f>
+        <v>11945.612244897959</v>
+      </c>
+      <c r="C2">
+        <f t="shared" si="0"/>
+        <v>118.44897959183673</v>
+      </c>
+      <c r="D2">
+        <f t="shared" si="0"/>
+        <v>113.42658430612244</v>
+      </c>
+      <c r="E2">
+        <f t="shared" si="0"/>
+        <v>11221.693877551021</v>
+      </c>
+      <c r="F2">
+        <f t="shared" si="0"/>
+        <v>111</v>
+      </c>
+      <c r="G2">
+        <f t="shared" si="0"/>
+        <v>113.88519681632653</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3">
+        <v>10212</v>
+      </c>
+      <c r="C3">
+        <v>405</v>
+      </c>
+      <c r="D3">
+        <v>136.5643</v>
+      </c>
+      <c r="E3">
+        <v>6822</v>
+      </c>
+      <c r="F3">
+        <v>26</v>
+      </c>
+      <c r="G3">
+        <v>136.5643</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>11870</v>
+      </c>
+      <c r="C4">
+        <v>32</v>
+      </c>
+      <c r="D4">
+        <v>129.40009000000001</v>
+      </c>
+      <c r="E4">
+        <v>6883</v>
+      </c>
+      <c r="F4">
+        <v>21</v>
+      </c>
+      <c r="G4">
+        <v>129.40009000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>9984</v>
+      </c>
+      <c r="C5">
+        <v>18</v>
+      </c>
+      <c r="D5">
+        <v>115.53062</v>
+      </c>
+      <c r="E5">
+        <v>6972</v>
+      </c>
+      <c r="F5">
+        <v>11</v>
+      </c>
+      <c r="G5">
+        <v>115.53062</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>15636</v>
+      </c>
+      <c r="C6">
+        <v>88</v>
+      </c>
+      <c r="D6">
+        <v>156.55205000000001</v>
+      </c>
+      <c r="E6">
+        <v>15433</v>
+      </c>
+      <c r="F6">
+        <v>48</v>
+      </c>
+      <c r="G6">
+        <v>156.55205000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>3145</v>
+      </c>
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7">
+        <v>76.556359999999998</v>
+      </c>
+      <c r="E7">
+        <v>2263</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>76.556359999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>15487</v>
+      </c>
+      <c r="C8">
+        <v>28</v>
+      </c>
+      <c r="D8">
+        <v>135.94968</v>
+      </c>
+      <c r="E8">
+        <v>15638</v>
+      </c>
+      <c r="F8">
+        <v>30</v>
+      </c>
+      <c r="G8">
+        <v>135.94968</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>9746</v>
+      </c>
+      <c r="C9">
+        <v>22</v>
+      </c>
+      <c r="D9">
+        <v>136.24876</v>
+      </c>
+      <c r="E9">
+        <v>6965</v>
+      </c>
+      <c r="F9">
+        <v>13</v>
+      </c>
+      <c r="G9">
+        <v>136.24876</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>12390</v>
+      </c>
+      <c r="C10">
+        <v>25</v>
+      </c>
+      <c r="D10">
+        <v>148.29958999999999</v>
+      </c>
+      <c r="E10">
+        <v>8376</v>
+      </c>
+      <c r="F10">
+        <v>14</v>
+      </c>
+      <c r="G10">
+        <v>148.29958999999999</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>15720</v>
+      </c>
+      <c r="C11">
+        <v>92</v>
+      </c>
+      <c r="D11">
+        <v>178.80206000000001</v>
+      </c>
+      <c r="E11">
+        <v>15696</v>
+      </c>
+      <c r="F11">
+        <v>49</v>
+      </c>
+      <c r="G11">
+        <v>178.80206000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12">
+        <v>12118</v>
+      </c>
+      <c r="C12">
+        <v>25</v>
+      </c>
+      <c r="D12">
+        <v>116.12376399999999</v>
+      </c>
+      <c r="E12">
+        <v>8914</v>
+      </c>
+      <c r="F12">
+        <v>16</v>
+      </c>
+      <c r="G12">
+        <v>116.12376399999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>15707</v>
+      </c>
+      <c r="C13">
+        <v>104</v>
+      </c>
+      <c r="D13">
+        <v>141.29163</v>
+      </c>
+      <c r="E13">
+        <v>15692</v>
+      </c>
+      <c r="F13">
+        <v>261</v>
+      </c>
+      <c r="G13">
+        <v>141.29163</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>15666</v>
+      </c>
+      <c r="C14">
+        <v>71</v>
+      </c>
+      <c r="D14">
+        <v>151.76651000000001</v>
+      </c>
+      <c r="E14">
+        <v>15671</v>
+      </c>
+      <c r="F14">
+        <v>72</v>
+      </c>
+      <c r="G14">
+        <v>152.2518</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>3093</v>
+      </c>
+      <c r="C15">
+        <v>5</v>
+      </c>
+      <c r="D15">
+        <v>52.931980000000003</v>
+      </c>
+      <c r="E15">
+        <v>2266</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <v>53.096195000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>14548</v>
+      </c>
+      <c r="C16">
+        <v>42</v>
+      </c>
+      <c r="D16">
+        <v>153.33760000000001</v>
+      </c>
+      <c r="E16">
+        <v>12480</v>
+      </c>
+      <c r="F16">
+        <v>27</v>
+      </c>
+      <c r="G16">
+        <v>153.33760000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>5503</v>
+      </c>
+      <c r="C17">
+        <v>16</v>
+      </c>
+      <c r="D17">
+        <v>59.174619999999997</v>
+      </c>
+      <c r="E17">
+        <v>5138</v>
+      </c>
+      <c r="F17">
+        <v>18</v>
+      </c>
+      <c r="G17">
+        <v>59.174619999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>14544</v>
+      </c>
+      <c r="C18">
+        <v>213</v>
+      </c>
+      <c r="D18">
+        <v>123.65992</v>
+      </c>
+      <c r="E18">
+        <v>14557</v>
+      </c>
+      <c r="F18">
+        <v>81</v>
+      </c>
+      <c r="G18">
+        <v>124.14521000000001</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>12919</v>
+      </c>
+      <c r="C19">
+        <v>25</v>
+      </c>
+      <c r="D19">
+        <v>74.881739999999994</v>
+      </c>
+      <c r="E19">
+        <v>14385</v>
+      </c>
+      <c r="F19">
+        <v>28</v>
+      </c>
+      <c r="G19">
+        <v>74.881739999999994</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20">
+        <v>10719</v>
+      </c>
+      <c r="C20">
+        <v>16</v>
+      </c>
+      <c r="D20">
+        <v>107.22363</v>
+      </c>
+      <c r="E20">
+        <v>7488</v>
+      </c>
+      <c r="F20">
+        <v>11</v>
+      </c>
+      <c r="G20">
+        <v>107.22363</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21">
+        <v>5622</v>
+      </c>
+      <c r="C21">
+        <v>16</v>
+      </c>
+      <c r="D21">
+        <v>37.164214999999999</v>
+      </c>
+      <c r="E21">
+        <v>5299</v>
+      </c>
+      <c r="F21">
+        <v>18</v>
+      </c>
+      <c r="G21">
+        <v>37.164214999999999</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22">
+        <v>5840</v>
+      </c>
+      <c r="C22">
+        <v>15</v>
+      </c>
+      <c r="D22">
+        <v>44.235287</v>
+      </c>
+      <c r="E22">
+        <v>5637</v>
+      </c>
+      <c r="F22">
+        <v>17</v>
+      </c>
+      <c r="G22">
+        <v>43.656860000000002</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <v>7527</v>
+      </c>
+      <c r="C23">
+        <v>11</v>
+      </c>
+      <c r="D23">
+        <v>123.412964</v>
+      </c>
+      <c r="E23">
+        <v>6290</v>
+      </c>
+      <c r="F23">
+        <v>8</v>
+      </c>
+      <c r="G23">
+        <v>123.412964</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24">
+        <v>10171</v>
+      </c>
+      <c r="C24">
+        <v>16</v>
+      </c>
+      <c r="D24">
+        <v>112.07717</v>
+      </c>
+      <c r="E24">
+        <v>7147</v>
+      </c>
+      <c r="F24">
+        <v>9</v>
+      </c>
+      <c r="G24">
+        <v>114.21932</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <v>14498</v>
+      </c>
+      <c r="C25">
+        <v>30</v>
+      </c>
+      <c r="D25">
+        <v>94.038589999999999</v>
+      </c>
+      <c r="E25">
+        <v>15243</v>
+      </c>
+      <c r="F25">
+        <v>35</v>
+      </c>
+      <c r="G25">
+        <v>95.634789999999995</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26">
+        <v>13588</v>
+      </c>
+      <c r="C26">
+        <v>287</v>
+      </c>
+      <c r="D26">
+        <v>126.56553</v>
+      </c>
+      <c r="E26">
+        <v>13210</v>
+      </c>
+      <c r="F26">
+        <v>59</v>
+      </c>
+      <c r="G26">
+        <v>126.56553</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27">
+        <v>14103</v>
+      </c>
+      <c r="C27">
+        <v>24</v>
+      </c>
+      <c r="D27">
+        <v>91.710160000000002</v>
+      </c>
+      <c r="E27">
+        <v>14730</v>
+      </c>
+      <c r="F27">
+        <v>26</v>
+      </c>
+      <c r="G27">
+        <v>92.867019999999997</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28">
+        <v>13692</v>
+      </c>
+      <c r="C28">
+        <v>24</v>
+      </c>
+      <c r="D28">
+        <v>88.417270000000002</v>
+      </c>
+      <c r="E28">
+        <v>14450</v>
+      </c>
+      <c r="F28">
+        <v>182</v>
+      </c>
+      <c r="G28">
+        <v>89.574129999999997</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29">
+        <v>7367</v>
+      </c>
+      <c r="C29">
+        <v>10</v>
+      </c>
+      <c r="D29">
+        <v>118.38479</v>
+      </c>
+      <c r="E29">
+        <v>6075</v>
+      </c>
+      <c r="F29">
+        <v>8</v>
+      </c>
+      <c r="G29">
+        <v>119.21322000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30">
+        <v>11686</v>
+      </c>
+      <c r="C30">
+        <v>41</v>
+      </c>
+      <c r="D30">
+        <v>86.441153999999997</v>
+      </c>
+      <c r="E30">
+        <v>11367</v>
+      </c>
+      <c r="F30">
+        <v>48</v>
+      </c>
+      <c r="G30">
+        <v>89.161709999999999</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31">
+        <v>7256</v>
+      </c>
+      <c r="C31">
+        <v>10</v>
+      </c>
+      <c r="D31">
+        <v>125.127426</v>
+      </c>
+      <c r="E31">
+        <v>5879</v>
+      </c>
+      <c r="F31">
+        <v>204</v>
+      </c>
+      <c r="G31">
+        <v>125.127426</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32">
+        <v>7857</v>
+      </c>
+      <c r="C32">
+        <v>13</v>
+      </c>
+      <c r="D32">
+        <v>101.19113</v>
+      </c>
+      <c r="E32">
+        <v>6002</v>
+      </c>
+      <c r="F32">
+        <v>7</v>
+      </c>
+      <c r="G32">
+        <v>103.98278999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33">
+        <v>11889</v>
+      </c>
+      <c r="C33">
+        <v>36</v>
+      </c>
+      <c r="D33">
+        <v>96.486810000000006</v>
+      </c>
+      <c r="E33">
+        <v>12580</v>
+      </c>
+      <c r="F33">
+        <v>43</v>
+      </c>
+      <c r="G33">
+        <v>97.800529999999995</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34">
+        <v>15257</v>
+      </c>
+      <c r="C34">
+        <v>2877</v>
+      </c>
+      <c r="D34">
+        <v>101.69239</v>
+      </c>
+      <c r="E34">
+        <v>14274</v>
+      </c>
+      <c r="F34">
+        <v>70</v>
+      </c>
+      <c r="G34">
+        <v>101.69239</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35">
+        <v>15743</v>
+      </c>
+      <c r="C35">
+        <v>84</v>
+      </c>
+      <c r="D35">
+        <v>183.05538999999999</v>
+      </c>
+      <c r="E35">
+        <v>15743</v>
+      </c>
+      <c r="F35">
+        <v>73</v>
+      </c>
+      <c r="G35">
+        <v>185.02597</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36">
+        <v>11888</v>
+      </c>
+      <c r="C36">
+        <v>41</v>
+      </c>
+      <c r="D36">
+        <v>98.108130000000003</v>
+      </c>
+      <c r="E36">
+        <v>12579</v>
+      </c>
+      <c r="F36">
+        <v>33</v>
+      </c>
+      <c r="G36">
+        <v>98.764989999999997</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37">
+        <v>12052</v>
+      </c>
+      <c r="C37">
+        <v>24</v>
+      </c>
+      <c r="D37">
+        <v>108.12008</v>
+      </c>
+      <c r="E37">
+        <v>14000</v>
+      </c>
+      <c r="F37">
+        <v>32</v>
+      </c>
+      <c r="G37">
+        <v>108.12008</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38">
+        <v>15703</v>
+      </c>
+      <c r="C38">
+        <v>72</v>
+      </c>
+      <c r="D38">
+        <v>164.22695999999999</v>
+      </c>
+      <c r="E38">
+        <v>15699</v>
+      </c>
+      <c r="F38">
+        <v>72</v>
+      </c>
+      <c r="G38">
+        <v>164.71960000000001</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39">
+        <v>14629</v>
+      </c>
+      <c r="C39">
+        <v>56</v>
+      </c>
+      <c r="D39">
+        <v>92.363960000000006</v>
+      </c>
+      <c r="E39">
+        <v>14486</v>
+      </c>
+      <c r="F39">
+        <v>3137</v>
+      </c>
+      <c r="G39">
+        <v>92.363960000000006</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40">
+        <v>14877</v>
+      </c>
+      <c r="C40">
+        <v>29</v>
+      </c>
+      <c r="D40">
+        <v>109.57259999999999</v>
+      </c>
+      <c r="E40">
+        <v>14638</v>
+      </c>
+      <c r="F40">
+        <v>29</v>
+      </c>
+      <c r="G40">
+        <v>110.80636</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41">
+        <v>5443</v>
+      </c>
+      <c r="C41">
+        <v>8</v>
+      </c>
+      <c r="D41">
+        <v>95.363969999999995</v>
+      </c>
+      <c r="E41">
+        <v>4208</v>
+      </c>
+      <c r="F41">
+        <v>5</v>
+      </c>
+      <c r="G41">
+        <v>95.363969999999995</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42">
+        <v>15743</v>
+      </c>
+      <c r="C42">
+        <v>88</v>
+      </c>
+      <c r="D42">
+        <v>164.12897000000001</v>
+      </c>
+      <c r="E42">
+        <v>15733</v>
+      </c>
+      <c r="F42">
+        <v>101</v>
+      </c>
+      <c r="G42">
+        <v>164.12897000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43">
+        <v>14795</v>
+      </c>
+      <c r="C43">
+        <v>370</v>
+      </c>
+      <c r="D43">
+        <v>117.98833500000001</v>
+      </c>
+      <c r="E43">
+        <v>14541</v>
+      </c>
+      <c r="F43">
+        <v>52</v>
+      </c>
+      <c r="G43">
+        <v>118.23098</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44">
+        <v>11297</v>
+      </c>
+      <c r="C44">
+        <v>19</v>
+      </c>
+      <c r="D44">
+        <v>123.150406</v>
+      </c>
+      <c r="E44">
+        <v>8635</v>
+      </c>
+      <c r="F44">
+        <v>15</v>
+      </c>
+      <c r="G44">
+        <v>124.95677000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45">
+        <v>15202</v>
+      </c>
+      <c r="C45">
+        <v>84</v>
+      </c>
+      <c r="D45">
+        <v>116.18226</v>
+      </c>
+      <c r="E45">
+        <v>15163</v>
+      </c>
+      <c r="F45">
+        <v>98</v>
+      </c>
+      <c r="G45">
+        <v>116.18226</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46">
+        <v>13725</v>
+      </c>
+      <c r="C46">
+        <v>35</v>
+      </c>
+      <c r="D46">
+        <v>81.069810000000004</v>
+      </c>
+      <c r="E46">
+        <v>15390</v>
+      </c>
+      <c r="F46">
+        <v>36</v>
+      </c>
+      <c r="G46">
+        <v>82.876170000000002</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47">
+        <v>15635</v>
+      </c>
+      <c r="C47">
+        <v>58</v>
+      </c>
+      <c r="D47">
+        <v>122.534294</v>
+      </c>
+      <c r="E47">
+        <v>15714</v>
+      </c>
+      <c r="F47">
+        <v>67</v>
+      </c>
+      <c r="G47">
+        <v>122.534294</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48">
+        <v>15735</v>
+      </c>
+      <c r="C48">
+        <v>38</v>
+      </c>
+      <c r="D48">
+        <v>137.98708999999999</v>
+      </c>
+      <c r="E48">
+        <v>15734</v>
+      </c>
+      <c r="F48">
+        <v>43</v>
+      </c>
+      <c r="G48">
+        <v>137.98708999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49">
+        <v>15628</v>
+      </c>
+      <c r="C49">
+        <v>50</v>
+      </c>
+      <c r="D49">
+        <v>135.40129999999999</v>
+      </c>
+      <c r="E49">
+        <v>15630</v>
+      </c>
+      <c r="F49">
+        <v>53</v>
+      </c>
+      <c r="G49">
+        <v>135.40129999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50">
+        <v>6228</v>
+      </c>
+      <c r="C50">
+        <v>18</v>
+      </c>
+      <c r="D50">
+        <v>53.087310000000002</v>
+      </c>
+      <c r="E50">
+        <v>6493</v>
+      </c>
+      <c r="F50">
+        <v>22</v>
+      </c>
+      <c r="G50">
+        <v>53.087310000000002</v>
+      </c>
+    </row>
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51">
+        <v>15652</v>
+      </c>
+      <c r="C51">
+        <v>89</v>
+      </c>
+      <c r="D51">
+        <v>114.32197600000001</v>
+      </c>
+      <c r="E51">
+        <v>15655</v>
+      </c>
+      <c r="F51">
+        <v>105</v>
+      </c>
+      <c r="G51">
+        <v>114.32197600000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52">
+        <v>9746</v>
+      </c>
+      <c r="C52">
+        <v>21</v>
+      </c>
+      <c r="D52">
+        <v>56.584519999999998</v>
+      </c>
+      <c r="E52">
+        <v>13734</v>
+      </c>
+      <c r="F52">
+        <v>29</v>
+      </c>
+      <c r="G52">
+        <v>57.405594000000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:M2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="5" width="12" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="12" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="16" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="17.42578125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="16" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="10.28515625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="12" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="12" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="15.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
@@ -966,51 +2210,51 @@
         <v>62</v>
       </c>
       <c r="B2">
-        <f>AVERAGE(B3:B51)</f>
+        <f t="shared" ref="B2:M2" si="0">AVERAGE(B3:B51)</f>
         <v>12274.836734693878</v>
       </c>
       <c r="C2">
-        <f>AVERAGE(C3:C51)</f>
+        <f t="shared" si="0"/>
         <v>69.040816326530617</v>
       </c>
       <c r="D2">
-        <f>AVERAGE(D3:D51)</f>
+        <f t="shared" si="0"/>
         <v>113.32909761224491</v>
       </c>
       <c r="E2">
-        <f>AVERAGE(E3:E51)</f>
+        <f t="shared" si="0"/>
         <v>9533.1632653061224</v>
       </c>
       <c r="F2">
-        <f>AVERAGE(F3:F51)</f>
+        <f t="shared" si="0"/>
         <v>5.8775510204081636</v>
       </c>
       <c r="G2">
-        <f>AVERAGE(G3:G51)</f>
+        <f t="shared" si="0"/>
         <v>113.32909761224491</v>
       </c>
       <c r="H2">
-        <f>AVERAGE(H3:H51)</f>
+        <f t="shared" si="0"/>
         <v>6628.5102040816328</v>
       </c>
       <c r="I2">
-        <f>AVERAGE(I3:I51)</f>
+        <f t="shared" si="0"/>
         <v>13.387755102040817</v>
       </c>
       <c r="J2">
-        <f>AVERAGE(J3:J51)</f>
+        <f t="shared" si="0"/>
         <v>113.99987018367345</v>
       </c>
       <c r="K2">
-        <f>AVERAGE(K3:K51)</f>
+        <f t="shared" si="0"/>
         <v>3700.8979591836733</v>
       </c>
       <c r="L2">
-        <f>AVERAGE(L3:L51)</f>
+        <f t="shared" si="0"/>
         <v>16.897959183673468</v>
       </c>
       <c r="M2">
-        <f>AVERAGE(M3:M51)</f>
+        <f t="shared" si="0"/>
         <v>117.22033489795922</v>
       </c>
     </row>
@@ -3070,7 +4314,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J51"/>
   <sheetViews>
@@ -3129,39 +4373,39 @@
         <v>62</v>
       </c>
       <c r="B2">
-        <f>AVERAGE(B3:B51)</f>
+        <f t="shared" ref="B2:J2" si="0">AVERAGE(B3:B51)</f>
         <v>1564.8367346938776</v>
       </c>
       <c r="C2">
-        <f>AVERAGE(C3:C51)</f>
+        <f t="shared" si="0"/>
         <v>6.795918367346939</v>
       </c>
       <c r="D2">
-        <f>AVERAGE(D3:D51)</f>
+        <f t="shared" si="0"/>
         <v>122.38346599999998</v>
       </c>
       <c r="E2">
-        <f>AVERAGE(E3:E51)</f>
+        <f t="shared" si="0"/>
         <v>140.32653061224491</v>
       </c>
       <c r="F2">
-        <f>AVERAGE(F3:F51)</f>
+        <f t="shared" si="0"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="G2">
-        <f>AVERAGE(G3:G51)</f>
+        <f t="shared" si="0"/>
         <v>170.29387751020408</v>
       </c>
       <c r="H2">
-        <f>AVERAGE(H3:H51)</f>
+        <f t="shared" si="0"/>
         <v>136.57142857142858</v>
       </c>
       <c r="I2">
-        <f>AVERAGE(I3:I51)</f>
+        <f t="shared" si="0"/>
         <v>0.16326530612244897</v>
       </c>
       <c r="J2">
-        <f>AVERAGE(J3:J51)</f>
+        <f t="shared" si="0"/>
         <v>172.78607261224488</v>
       </c>
     </row>
@@ -4731,1698 +5975,6 @@
       </c>
       <c r="J51">
         <v>98.870069999999998</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J52"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:J2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="10.28515625" customWidth="1"/>
-    <col min="2" max="6" width="14.7109375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>61</v>
-      </c>
-      <c r="B1" t="s">
-        <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D1" t="s">
-        <v>5</v>
-      </c>
-      <c r="E1" t="s">
-        <v>6</v>
-      </c>
-      <c r="F1" t="s">
-        <v>7</v>
-      </c>
-      <c r="G1" t="s">
-        <v>8</v>
-      </c>
-      <c r="H1" t="s">
-        <v>9</v>
-      </c>
-      <c r="I1" t="s">
-        <v>10</v>
-      </c>
-      <c r="J1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2">
-        <f>AVERAGE(B3:B51)</f>
-        <v>12177.65306122449</v>
-      </c>
-      <c r="C2">
-        <f>AVERAGE(C3:C51)</f>
-        <v>12.448979591836734</v>
-      </c>
-      <c r="D2">
-        <f>AVERAGE(D3:D51)</f>
-        <v>117.02324751020411</v>
-      </c>
-      <c r="E2">
-        <f>AVERAGE(E3:E51)</f>
-        <v>11984.714285714286</v>
-      </c>
-      <c r="F2">
-        <f>AVERAGE(F3:F51)</f>
-        <v>25.693877551020407</v>
-      </c>
-      <c r="G2">
-        <f>AVERAGE(G3:G51)</f>
-        <v>118.54178946938771</v>
-      </c>
-      <c r="H2">
-        <f>AVERAGE(H3:H51)</f>
-        <v>11779.408163265307</v>
-      </c>
-      <c r="I2">
-        <f>AVERAGE(I3:I51)</f>
-        <v>16.510204081632654</v>
-      </c>
-      <c r="J2">
-        <f>AVERAGE(J3:J51)</f>
-        <v>120.03179708163266</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B3">
-        <v>14214</v>
-      </c>
-      <c r="C3">
-        <v>50</v>
-      </c>
-      <c r="D3">
-        <v>136.5643</v>
-      </c>
-      <c r="E3">
-        <v>13825</v>
-      </c>
-      <c r="F3">
-        <v>15</v>
-      </c>
-      <c r="G3">
-        <v>136.5643</v>
-      </c>
-      <c r="H3">
-        <v>13285</v>
-      </c>
-      <c r="I3">
-        <v>13</v>
-      </c>
-      <c r="J3">
-        <v>136.5643</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4">
-        <v>14604</v>
-      </c>
-      <c r="C4">
-        <v>13</v>
-      </c>
-      <c r="D4">
-        <v>129.40009000000001</v>
-      </c>
-      <c r="E4">
-        <v>14269</v>
-      </c>
-      <c r="F4">
-        <v>541</v>
-      </c>
-      <c r="G4">
-        <v>129.40009000000001</v>
-      </c>
-      <c r="H4">
-        <v>13806</v>
-      </c>
-      <c r="I4">
-        <v>11</v>
-      </c>
-      <c r="J4">
-        <v>129.40009000000001</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5">
-        <v>13536</v>
-      </c>
-      <c r="C5">
-        <v>10</v>
-      </c>
-      <c r="D5">
-        <v>115.53062</v>
-      </c>
-      <c r="E5">
-        <v>13428</v>
-      </c>
-      <c r="F5">
-        <v>9</v>
-      </c>
-      <c r="G5">
-        <v>120.30083</v>
-      </c>
-      <c r="H5">
-        <v>13019</v>
-      </c>
-      <c r="I5">
-        <v>9</v>
-      </c>
-      <c r="J5">
-        <v>120.30083</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6">
-        <v>15643</v>
-      </c>
-      <c r="C6">
-        <v>10</v>
-      </c>
-      <c r="D6">
-        <v>156.38050000000001</v>
-      </c>
-      <c r="E6">
-        <v>15594</v>
-      </c>
-      <c r="F6">
-        <v>10</v>
-      </c>
-      <c r="G6">
-        <v>156.38050000000001</v>
-      </c>
-      <c r="H6">
-        <v>15515</v>
-      </c>
-      <c r="I6">
-        <v>11</v>
-      </c>
-      <c r="J6">
-        <v>156.38050000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7">
-        <v>5580</v>
-      </c>
-      <c r="C7">
-        <v>3</v>
-      </c>
-      <c r="D7">
-        <v>76.556359999999998</v>
-      </c>
-      <c r="E7">
-        <v>5477</v>
-      </c>
-      <c r="F7">
-        <v>3</v>
-      </c>
-      <c r="G7">
-        <v>76.556359999999998</v>
-      </c>
-      <c r="H7">
-        <v>5285</v>
-      </c>
-      <c r="I7">
-        <v>3</v>
-      </c>
-      <c r="J7">
-        <v>76.556359999999998</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8">
-        <v>14390</v>
-      </c>
-      <c r="C8">
-        <v>9</v>
-      </c>
-      <c r="D8">
-        <v>137.67151000000001</v>
-      </c>
-      <c r="E8">
-        <v>14386</v>
-      </c>
-      <c r="F8">
-        <v>9</v>
-      </c>
-      <c r="G8">
-        <v>138.08573999999999</v>
-      </c>
-      <c r="H8">
-        <v>14257</v>
-      </c>
-      <c r="I8">
-        <v>10</v>
-      </c>
-      <c r="J8">
-        <v>138.08573999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>17</v>
-      </c>
-      <c r="B9">
-        <v>14239</v>
-      </c>
-      <c r="C9">
-        <v>9</v>
-      </c>
-      <c r="D9">
-        <v>136.24876</v>
-      </c>
-      <c r="E9">
-        <v>13740</v>
-      </c>
-      <c r="F9">
-        <v>10</v>
-      </c>
-      <c r="G9">
-        <v>136.24876</v>
-      </c>
-      <c r="H9">
-        <v>13352</v>
-      </c>
-      <c r="I9">
-        <v>9</v>
-      </c>
-      <c r="J9">
-        <v>136.24876</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10">
-        <v>14870</v>
-      </c>
-      <c r="C10">
-        <v>9</v>
-      </c>
-      <c r="D10">
-        <v>148.13538</v>
-      </c>
-      <c r="E10">
-        <v>14584</v>
-      </c>
-      <c r="F10">
-        <v>9</v>
-      </c>
-      <c r="G10">
-        <v>148.13538</v>
-      </c>
-      <c r="H10">
-        <v>14146</v>
-      </c>
-      <c r="I10">
-        <v>9</v>
-      </c>
-      <c r="J10">
-        <v>148.13538</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>19</v>
-      </c>
-      <c r="B11">
-        <v>15710</v>
-      </c>
-      <c r="C11">
-        <v>11</v>
-      </c>
-      <c r="D11">
-        <v>178.80206000000001</v>
-      </c>
-      <c r="E11">
-        <v>15678</v>
-      </c>
-      <c r="F11">
-        <v>13</v>
-      </c>
-      <c r="G11">
-        <v>178.80206000000001</v>
-      </c>
-      <c r="H11">
-        <v>15627</v>
-      </c>
-      <c r="I11">
-        <v>13</v>
-      </c>
-      <c r="J11">
-        <v>178.80206000000001</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12">
-        <v>14177</v>
-      </c>
-      <c r="C12">
-        <v>9</v>
-      </c>
-      <c r="D12">
-        <v>116.12376399999999</v>
-      </c>
-      <c r="E12">
-        <v>13998</v>
-      </c>
-      <c r="F12">
-        <v>9</v>
-      </c>
-      <c r="G12">
-        <v>118.5153</v>
-      </c>
-      <c r="H12">
-        <v>13648</v>
-      </c>
-      <c r="I12">
-        <v>9</v>
-      </c>
-      <c r="J12">
-        <v>118.5153</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13">
-        <v>15633</v>
-      </c>
-      <c r="C13">
-        <v>9</v>
-      </c>
-      <c r="D13">
-        <v>150.3664</v>
-      </c>
-      <c r="E13">
-        <v>15562</v>
-      </c>
-      <c r="F13">
-        <v>10</v>
-      </c>
-      <c r="G13">
-        <v>155.01094000000001</v>
-      </c>
-      <c r="H13">
-        <v>15426</v>
-      </c>
-      <c r="I13">
-        <v>11</v>
-      </c>
-      <c r="J13">
-        <v>155.62860000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>21</v>
-      </c>
-      <c r="B14">
-        <v>15487</v>
-      </c>
-      <c r="C14">
-        <v>108</v>
-      </c>
-      <c r="D14">
-        <v>162.87009</v>
-      </c>
-      <c r="E14">
-        <v>15298</v>
-      </c>
-      <c r="F14">
-        <v>9</v>
-      </c>
-      <c r="G14">
-        <v>162.87009</v>
-      </c>
-      <c r="H14">
-        <v>15118</v>
-      </c>
-      <c r="I14">
-        <v>9</v>
-      </c>
-      <c r="J14">
-        <v>162.87009</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>22</v>
-      </c>
-      <c r="B15">
-        <v>5738</v>
-      </c>
-      <c r="C15">
-        <v>3</v>
-      </c>
-      <c r="D15">
-        <v>68.710160000000002</v>
-      </c>
-      <c r="E15">
-        <v>5935</v>
-      </c>
-      <c r="F15">
-        <v>3</v>
-      </c>
-      <c r="G15">
-        <v>72.445440000000005</v>
-      </c>
-      <c r="H15">
-        <v>6412</v>
-      </c>
-      <c r="I15">
-        <v>3</v>
-      </c>
-      <c r="J15">
-        <v>78.395195000000001</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>23</v>
-      </c>
-      <c r="B16">
-        <v>15479</v>
-      </c>
-      <c r="C16">
-        <v>10</v>
-      </c>
-      <c r="D16">
-        <v>165.11578</v>
-      </c>
-      <c r="E16">
-        <v>15372</v>
-      </c>
-      <c r="F16">
-        <v>9</v>
-      </c>
-      <c r="G16">
-        <v>168.84616</v>
-      </c>
-      <c r="H16">
-        <v>15241</v>
-      </c>
-      <c r="I16">
-        <v>9</v>
-      </c>
-      <c r="J16">
-        <v>170.17458999999999</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>24</v>
-      </c>
-      <c r="B17">
-        <v>6543</v>
-      </c>
-      <c r="C17">
-        <v>4</v>
-      </c>
-      <c r="D17">
-        <v>74.913579999999996</v>
-      </c>
-      <c r="E17">
-        <v>6932</v>
-      </c>
-      <c r="F17">
-        <v>4</v>
-      </c>
-      <c r="G17">
-        <v>78.570440000000005</v>
-      </c>
-      <c r="H17">
-        <v>7543</v>
-      </c>
-      <c r="I17">
-        <v>4</v>
-      </c>
-      <c r="J17">
-        <v>84.145189999999999</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>25</v>
-      </c>
-      <c r="B18">
-        <v>13548</v>
-      </c>
-      <c r="C18">
-        <v>9</v>
-      </c>
-      <c r="D18">
-        <v>133.7886</v>
-      </c>
-      <c r="E18">
-        <v>12788</v>
-      </c>
-      <c r="F18">
-        <v>8</v>
-      </c>
-      <c r="G18">
-        <v>133.7886</v>
-      </c>
-      <c r="H18">
-        <v>12296</v>
-      </c>
-      <c r="I18">
-        <v>8</v>
-      </c>
-      <c r="J18">
-        <v>133.7886</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>26</v>
-      </c>
-      <c r="B19">
-        <v>8123</v>
-      </c>
-      <c r="C19">
-        <v>5</v>
-      </c>
-      <c r="D19">
-        <v>86.495699999999999</v>
-      </c>
-      <c r="E19">
-        <v>7806</v>
-      </c>
-      <c r="F19">
-        <v>5</v>
-      </c>
-      <c r="G19">
-        <v>91.449119999999994</v>
-      </c>
-      <c r="H19">
-        <v>7861</v>
-      </c>
-      <c r="I19">
-        <v>5</v>
-      </c>
-      <c r="J19">
-        <v>99.559399999999997</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>27</v>
-      </c>
-      <c r="B20">
-        <v>13284</v>
-      </c>
-      <c r="C20">
-        <v>9</v>
-      </c>
-      <c r="D20">
-        <v>115.73344</v>
-      </c>
-      <c r="E20">
-        <v>13113</v>
-      </c>
-      <c r="F20">
-        <v>140</v>
-      </c>
-      <c r="G20">
-        <v>115.73344</v>
-      </c>
-      <c r="H20">
-        <v>12908</v>
-      </c>
-      <c r="I20">
-        <v>9</v>
-      </c>
-      <c r="J20">
-        <v>116.8903</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>28</v>
-      </c>
-      <c r="B21">
-        <v>6583</v>
-      </c>
-      <c r="C21">
-        <v>4</v>
-      </c>
-      <c r="D21">
-        <v>53.231605999999999</v>
-      </c>
-      <c r="E21">
-        <v>6966</v>
-      </c>
-      <c r="F21">
-        <v>5</v>
-      </c>
-      <c r="G21">
-        <v>56.888460000000002</v>
-      </c>
-      <c r="H21">
-        <v>7802</v>
-      </c>
-      <c r="I21">
-        <v>4</v>
-      </c>
-      <c r="J21">
-        <v>63.798996000000002</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>29</v>
-      </c>
-      <c r="B22">
-        <v>7058</v>
-      </c>
-      <c r="C22">
-        <v>4</v>
-      </c>
-      <c r="D22">
-        <v>59.724249999999998</v>
-      </c>
-      <c r="E22">
-        <v>7549</v>
-      </c>
-      <c r="F22">
-        <v>5</v>
-      </c>
-      <c r="G22">
-        <v>63.381104000000001</v>
-      </c>
-      <c r="H22">
-        <v>8024</v>
-      </c>
-      <c r="I22">
-        <v>4</v>
-      </c>
-      <c r="J22">
-        <v>66.863960000000006</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>30</v>
-      </c>
-      <c r="B23">
-        <v>10462</v>
-      </c>
-      <c r="C23">
-        <v>6</v>
-      </c>
-      <c r="D23">
-        <v>123.20586</v>
-      </c>
-      <c r="E23">
-        <v>10137</v>
-      </c>
-      <c r="F23">
-        <v>7</v>
-      </c>
-      <c r="G23">
-        <v>123.20586</v>
-      </c>
-      <c r="H23">
-        <v>9929</v>
-      </c>
-      <c r="I23">
-        <v>6</v>
-      </c>
-      <c r="J23">
-        <v>123.20586</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B24">
-        <v>12712</v>
-      </c>
-      <c r="C24">
-        <v>9</v>
-      </c>
-      <c r="D24">
-        <v>111.91296</v>
-      </c>
-      <c r="E24">
-        <v>12297</v>
-      </c>
-      <c r="F24">
-        <v>8</v>
-      </c>
-      <c r="G24">
-        <v>111.91296</v>
-      </c>
-      <c r="H24">
-        <v>12009</v>
-      </c>
-      <c r="I24">
-        <v>9</v>
-      </c>
-      <c r="J24">
-        <v>111.91296</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>32</v>
-      </c>
-      <c r="B25">
-        <v>10390</v>
-      </c>
-      <c r="C25">
-        <v>7</v>
-      </c>
-      <c r="D25">
-        <v>93.545950000000005</v>
-      </c>
-      <c r="E25">
-        <v>9950</v>
-      </c>
-      <c r="F25">
-        <v>7</v>
-      </c>
-      <c r="G25">
-        <v>93.545950000000005</v>
-      </c>
-      <c r="H25">
-        <v>9612</v>
-      </c>
-      <c r="I25">
-        <v>6</v>
-      </c>
-      <c r="J25">
-        <v>93.545950000000005</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>33</v>
-      </c>
-      <c r="B26">
-        <v>14235</v>
-      </c>
-      <c r="C26">
-        <v>13</v>
-      </c>
-      <c r="D26">
-        <v>126.62743</v>
-      </c>
-      <c r="E26">
-        <v>13987</v>
-      </c>
-      <c r="F26">
-        <v>12</v>
-      </c>
-      <c r="G26">
-        <v>126.62743</v>
-      </c>
-      <c r="H26">
-        <v>13725</v>
-      </c>
-      <c r="I26">
-        <v>299</v>
-      </c>
-      <c r="J26">
-        <v>126.62743</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27">
-        <v>9017</v>
-      </c>
-      <c r="C27">
-        <v>6</v>
-      </c>
-      <c r="D27">
-        <v>91.545944000000006</v>
-      </c>
-      <c r="E27">
-        <v>8358</v>
-      </c>
-      <c r="F27">
-        <v>6</v>
-      </c>
-      <c r="G27">
-        <v>91.545944000000006</v>
-      </c>
-      <c r="H27">
-        <v>7695</v>
-      </c>
-      <c r="I27">
-        <v>5</v>
-      </c>
-      <c r="J27">
-        <v>91.545944000000006</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>35</v>
-      </c>
-      <c r="B28">
-        <v>8120</v>
-      </c>
-      <c r="C28">
-        <v>5</v>
-      </c>
-      <c r="D28">
-        <v>88.045944000000006</v>
-      </c>
-      <c r="E28">
-        <v>7404</v>
-      </c>
-      <c r="F28">
-        <v>4</v>
-      </c>
-      <c r="G28">
-        <v>88.045944000000006</v>
-      </c>
-      <c r="H28">
-        <v>6822</v>
-      </c>
-      <c r="I28">
-        <v>5</v>
-      </c>
-      <c r="J28">
-        <v>88.045944000000006</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>36</v>
-      </c>
-      <c r="B29">
-        <v>9992</v>
-      </c>
-      <c r="C29">
-        <v>6</v>
-      </c>
-      <c r="D29">
-        <v>118.38479</v>
-      </c>
-      <c r="E29">
-        <v>9588</v>
-      </c>
-      <c r="F29">
-        <v>189</v>
-      </c>
-      <c r="G29">
-        <v>118.38479</v>
-      </c>
-      <c r="H29">
-        <v>9300</v>
-      </c>
-      <c r="I29">
-        <v>6</v>
-      </c>
-      <c r="J29">
-        <v>118.38479</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>37</v>
-      </c>
-      <c r="B30">
-        <v>9554</v>
-      </c>
-      <c r="C30">
-        <v>11</v>
-      </c>
-      <c r="D30">
-        <v>86.441149999999993</v>
-      </c>
-      <c r="E30">
-        <v>9146</v>
-      </c>
-      <c r="F30">
-        <v>12</v>
-      </c>
-      <c r="G30">
-        <v>86.441149999999993</v>
-      </c>
-      <c r="H30">
-        <v>8761</v>
-      </c>
-      <c r="I30">
-        <v>9</v>
-      </c>
-      <c r="J30">
-        <v>86.441149999999993</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>38</v>
-      </c>
-      <c r="B31">
-        <v>10198</v>
-      </c>
-      <c r="C31">
-        <v>6</v>
-      </c>
-      <c r="D31">
-        <v>125.127426</v>
-      </c>
-      <c r="E31">
-        <v>9784</v>
-      </c>
-      <c r="F31">
-        <v>9</v>
-      </c>
-      <c r="G31">
-        <v>125.127426</v>
-      </c>
-      <c r="H31">
-        <v>9473</v>
-      </c>
-      <c r="I31">
-        <v>6</v>
-      </c>
-      <c r="J31">
-        <v>125.127426</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>39</v>
-      </c>
-      <c r="B32">
-        <v>11718</v>
-      </c>
-      <c r="C32">
-        <v>13</v>
-      </c>
-      <c r="D32">
-        <v>101.19113</v>
-      </c>
-      <c r="E32">
-        <v>11192</v>
-      </c>
-      <c r="F32">
-        <v>11</v>
-      </c>
-      <c r="G32">
-        <v>101.19113</v>
-      </c>
-      <c r="H32">
-        <v>10770</v>
-      </c>
-      <c r="I32">
-        <v>13</v>
-      </c>
-      <c r="J32">
-        <v>101.19113</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>40</v>
-      </c>
-      <c r="B33">
-        <v>8478</v>
-      </c>
-      <c r="C33">
-        <v>6</v>
-      </c>
-      <c r="D33">
-        <v>96.322599999999994</v>
-      </c>
-      <c r="E33">
-        <v>8112</v>
-      </c>
-      <c r="F33">
-        <v>5</v>
-      </c>
-      <c r="G33">
-        <v>96.322599999999994</v>
-      </c>
-      <c r="H33">
-        <v>7749</v>
-      </c>
-      <c r="I33">
-        <v>6</v>
-      </c>
-      <c r="J33">
-        <v>96.322599999999994</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>41</v>
-      </c>
-      <c r="B34">
-        <v>14380</v>
-      </c>
-      <c r="C34">
-        <v>13</v>
-      </c>
-      <c r="D34">
-        <v>119.948494</v>
-      </c>
-      <c r="E34">
-        <v>14415</v>
-      </c>
-      <c r="F34">
-        <v>14</v>
-      </c>
-      <c r="G34">
-        <v>127.058784</v>
-      </c>
-      <c r="H34">
-        <v>14453</v>
-      </c>
-      <c r="I34">
-        <v>14</v>
-      </c>
-      <c r="J34">
-        <v>134.91539</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>42</v>
-      </c>
-      <c r="B35">
-        <v>15727</v>
-      </c>
-      <c r="C35">
-        <v>14</v>
-      </c>
-      <c r="D35">
-        <v>183.05538999999999</v>
-      </c>
-      <c r="E35">
-        <v>15684</v>
-      </c>
-      <c r="F35">
-        <v>11</v>
-      </c>
-      <c r="G35">
-        <v>183.05538999999999</v>
-      </c>
-      <c r="H35">
-        <v>15615</v>
-      </c>
-      <c r="I35">
-        <v>15</v>
-      </c>
-      <c r="J35">
-        <v>183.38381999999999</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
-        <v>43</v>
-      </c>
-      <c r="B36">
-        <v>8470</v>
-      </c>
-      <c r="C36">
-        <v>7</v>
-      </c>
-      <c r="D36">
-        <v>97.943923999999996</v>
-      </c>
-      <c r="E36">
-        <v>8102</v>
-      </c>
-      <c r="F36">
-        <v>7</v>
-      </c>
-      <c r="G36">
-        <v>97.943923999999996</v>
-      </c>
-      <c r="H36">
-        <v>7731</v>
-      </c>
-      <c r="I36">
-        <v>10</v>
-      </c>
-      <c r="J36">
-        <v>97.943923999999996</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>44</v>
-      </c>
-      <c r="B37">
-        <v>7363</v>
-      </c>
-      <c r="C37">
-        <v>6</v>
-      </c>
-      <c r="D37">
-        <v>107.95586400000001</v>
-      </c>
-      <c r="E37">
-        <v>6908</v>
-      </c>
-      <c r="F37">
-        <v>7</v>
-      </c>
-      <c r="G37">
-        <v>107.95586400000001</v>
-      </c>
-      <c r="H37">
-        <v>6591</v>
-      </c>
-      <c r="I37">
-        <v>5</v>
-      </c>
-      <c r="J37">
-        <v>107.95586400000001</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>45</v>
-      </c>
-      <c r="B38">
-        <v>15693</v>
-      </c>
-      <c r="C38">
-        <v>10</v>
-      </c>
-      <c r="D38">
-        <v>164.22695999999999</v>
-      </c>
-      <c r="E38">
-        <v>15634</v>
-      </c>
-      <c r="F38">
-        <v>11</v>
-      </c>
-      <c r="G38">
-        <v>164.22695999999999</v>
-      </c>
-      <c r="H38">
-        <v>15554</v>
-      </c>
-      <c r="I38">
-        <v>11</v>
-      </c>
-      <c r="J38">
-        <v>164.55538999999999</v>
-      </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>46</v>
-      </c>
-      <c r="B39">
-        <v>14345</v>
-      </c>
-      <c r="C39">
-        <v>9</v>
-      </c>
-      <c r="D39">
-        <v>110.62006</v>
-      </c>
-      <c r="E39">
-        <v>14431</v>
-      </c>
-      <c r="F39">
-        <v>10</v>
-      </c>
-      <c r="G39">
-        <v>117.73035400000001</v>
-      </c>
-      <c r="H39">
-        <v>14500</v>
-      </c>
-      <c r="I39">
-        <v>11</v>
-      </c>
-      <c r="J39">
-        <v>125.58696</v>
-      </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>47</v>
-      </c>
-      <c r="B40">
-        <v>13355</v>
-      </c>
-      <c r="C40">
-        <v>10</v>
-      </c>
-      <c r="D40">
-        <v>109.36548999999999</v>
-      </c>
-      <c r="E40">
-        <v>12340</v>
-      </c>
-      <c r="F40">
-        <v>8</v>
-      </c>
-      <c r="G40">
-        <v>109.36548999999999</v>
-      </c>
-      <c r="H40">
-        <v>11369</v>
-      </c>
-      <c r="I40">
-        <v>9</v>
-      </c>
-      <c r="J40">
-        <v>109.36548999999999</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>48</v>
-      </c>
-      <c r="B41">
-        <v>13542</v>
-      </c>
-      <c r="C41">
-        <v>9</v>
-      </c>
-      <c r="D41">
-        <v>110.10903999999999</v>
-      </c>
-      <c r="E41">
-        <v>14419</v>
-      </c>
-      <c r="F41">
-        <v>9</v>
-      </c>
-      <c r="G41">
-        <v>123.26957</v>
-      </c>
-      <c r="H41">
-        <v>14550</v>
-      </c>
-      <c r="I41">
-        <v>11</v>
-      </c>
-      <c r="J41">
-        <v>130.99446</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>49</v>
-      </c>
-      <c r="B42">
-        <v>15727</v>
-      </c>
-      <c r="C42">
-        <v>10</v>
-      </c>
-      <c r="D42">
-        <v>164.6412</v>
-      </c>
-      <c r="E42">
-        <v>15670</v>
-      </c>
-      <c r="F42">
-        <v>11</v>
-      </c>
-      <c r="G42">
-        <v>164.80542</v>
-      </c>
-      <c r="H42">
-        <v>15584</v>
-      </c>
-      <c r="I42">
-        <v>10</v>
-      </c>
-      <c r="J42">
-        <v>165.46227999999999</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>50</v>
-      </c>
-      <c r="B43">
-        <v>14980</v>
-      </c>
-      <c r="C43">
-        <v>10</v>
-      </c>
-      <c r="D43">
-        <v>117.98833999999999</v>
-      </c>
-      <c r="E43">
-        <v>14851</v>
-      </c>
-      <c r="F43">
-        <v>10</v>
-      </c>
-      <c r="G43">
-        <v>121.02388000000001</v>
-      </c>
-      <c r="H43">
-        <v>14993</v>
-      </c>
-      <c r="I43">
-        <v>10</v>
-      </c>
-      <c r="J43">
-        <v>128.97210000000001</v>
-      </c>
-    </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>51</v>
-      </c>
-      <c r="B44">
-        <v>14023</v>
-      </c>
-      <c r="C44">
-        <v>66</v>
-      </c>
-      <c r="D44">
-        <v>123.150406</v>
-      </c>
-      <c r="E44">
-        <v>13750</v>
-      </c>
-      <c r="F44">
-        <v>8</v>
-      </c>
-      <c r="G44">
-        <v>123.150406</v>
-      </c>
-      <c r="H44">
-        <v>13709</v>
-      </c>
-      <c r="I44">
-        <v>9</v>
-      </c>
-      <c r="J44">
-        <v>124.79255999999999</v>
-      </c>
-    </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>52</v>
-      </c>
-      <c r="B45">
-        <v>14932</v>
-      </c>
-      <c r="C45">
-        <v>10</v>
-      </c>
-      <c r="D45">
-        <v>116.18226</v>
-      </c>
-      <c r="E45">
-        <v>14517</v>
-      </c>
-      <c r="F45">
-        <v>9</v>
-      </c>
-      <c r="G45">
-        <v>116.18226</v>
-      </c>
-      <c r="H45">
-        <v>14178</v>
-      </c>
-      <c r="I45">
-        <v>9</v>
-      </c>
-      <c r="J45">
-        <v>116.34647</v>
-      </c>
-    </row>
-    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>53</v>
-      </c>
-      <c r="B46">
-        <v>8241</v>
-      </c>
-      <c r="C46">
-        <v>5</v>
-      </c>
-      <c r="D46">
-        <v>81.069810000000004</v>
-      </c>
-      <c r="E46">
-        <v>7887</v>
-      </c>
-      <c r="F46">
-        <v>4</v>
-      </c>
-      <c r="G46">
-        <v>81.069810000000004</v>
-      </c>
-      <c r="H46">
-        <v>7512</v>
-      </c>
-      <c r="I46">
-        <v>5</v>
-      </c>
-      <c r="J46">
-        <v>81.069810000000004</v>
-      </c>
-    </row>
-    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>54</v>
-      </c>
-      <c r="B47">
-        <v>14898</v>
-      </c>
-      <c r="C47">
-        <v>9</v>
-      </c>
-      <c r="D47">
-        <v>122.534294</v>
-      </c>
-      <c r="E47">
-        <v>14621</v>
-      </c>
-      <c r="F47">
-        <v>10</v>
-      </c>
-      <c r="G47">
-        <v>122.534294</v>
-      </c>
-      <c r="H47">
-        <v>12710</v>
-      </c>
-      <c r="I47">
-        <v>114</v>
-      </c>
-      <c r="J47">
-        <v>122.534294</v>
-      </c>
-    </row>
-    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>55</v>
-      </c>
-      <c r="B48">
-        <v>15606</v>
-      </c>
-      <c r="C48">
-        <v>10</v>
-      </c>
-      <c r="D48">
-        <v>137.98708999999999</v>
-      </c>
-      <c r="E48">
-        <v>15268</v>
-      </c>
-      <c r="F48">
-        <v>10</v>
-      </c>
-      <c r="G48">
-        <v>137.98708999999999</v>
-      </c>
-      <c r="H48">
-        <v>15013</v>
-      </c>
-      <c r="I48">
-        <v>9</v>
-      </c>
-      <c r="J48">
-        <v>137.98708999999999</v>
-      </c>
-    </row>
-    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
-        <v>56</v>
-      </c>
-      <c r="B49">
-        <v>15564</v>
-      </c>
-      <c r="C49">
-        <v>12</v>
-      </c>
-      <c r="D49">
-        <v>135.40129999999999</v>
-      </c>
-      <c r="E49">
-        <v>15477</v>
-      </c>
-      <c r="F49">
-        <v>10</v>
-      </c>
-      <c r="G49">
-        <v>135.40129999999999</v>
-      </c>
-      <c r="H49">
-        <v>15047</v>
-      </c>
-      <c r="I49">
-        <v>10</v>
-      </c>
-      <c r="J49">
-        <v>135.40129999999999</v>
-      </c>
-    </row>
-    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>57</v>
-      </c>
-      <c r="B50">
-        <v>5273</v>
-      </c>
-      <c r="C50">
-        <v>4</v>
-      </c>
-      <c r="D50">
-        <v>52.923096000000001</v>
-      </c>
-      <c r="E50">
-        <v>6058</v>
-      </c>
-      <c r="F50">
-        <v>4</v>
-      </c>
-      <c r="G50">
-        <v>61.101399999999998</v>
-      </c>
-      <c r="H50">
-        <v>7111</v>
-      </c>
-      <c r="I50">
-        <v>4</v>
-      </c>
-      <c r="J50">
-        <v>66.474239999999995</v>
-      </c>
-    </row>
-    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>58</v>
-      </c>
-      <c r="B51">
-        <v>15271</v>
-      </c>
-      <c r="C51">
-        <v>10</v>
-      </c>
-      <c r="D51">
-        <v>114.32197600000001</v>
-      </c>
-      <c r="E51">
-        <v>14964</v>
-      </c>
-      <c r="F51">
-        <v>10</v>
-      </c>
-      <c r="G51">
-        <v>114.36118999999999</v>
-      </c>
-      <c r="H51">
-        <v>14555</v>
-      </c>
-      <c r="I51">
-        <v>10</v>
-      </c>
-      <c r="J51">
-        <v>114.36118999999999</v>
-      </c>
-    </row>
-    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>59</v>
-      </c>
-      <c r="B52">
-        <v>6704</v>
-      </c>
-      <c r="C52">
-        <v>4</v>
-      </c>
-      <c r="D52">
-        <v>56.584519999999998</v>
-      </c>
-      <c r="E52">
-        <v>6352</v>
-      </c>
-      <c r="F52">
-        <v>4</v>
-      </c>
-      <c r="G52">
-        <v>56.584519999999998</v>
-      </c>
-      <c r="H52">
-        <v>5900</v>
-      </c>
-      <c r="I52">
-        <v>4</v>
-      </c>
-      <c r="J52">
-        <v>56.584519999999998</v>
       </c>
     </row>
   </sheetData>
@@ -6487,39 +6039,39 @@
         <v>62</v>
       </c>
       <c r="B2">
-        <f>AVERAGE(B3:B51)</f>
+        <f t="shared" ref="B2:J2" si="0">AVERAGE(B3:B51)</f>
         <v>9444.2040816326535</v>
       </c>
       <c r="C2">
-        <f>AVERAGE(C3:C51)</f>
+        <f t="shared" si="0"/>
         <v>9.5306122448979593</v>
       </c>
       <c r="D2">
-        <f>AVERAGE(D3:D51)</f>
+        <f t="shared" si="0"/>
         <v>120.31054802040812</v>
       </c>
       <c r="E2">
-        <f>AVERAGE(E3:E51)</f>
+        <f t="shared" si="0"/>
         <v>7708.8163265306121</v>
       </c>
       <c r="F2">
-        <f>AVERAGE(F3:F51)</f>
+        <f t="shared" si="0"/>
         <v>6.1020408163265305</v>
       </c>
       <c r="G2">
-        <f>AVERAGE(G3:G51)</f>
+        <f t="shared" si="0"/>
         <v>144.12979475510201</v>
       </c>
       <c r="H2">
-        <f>AVERAGE(H3:H51)</f>
+        <f t="shared" si="0"/>
         <v>7261</v>
       </c>
       <c r="I2">
-        <f>AVERAGE(I3:I51)</f>
+        <f t="shared" si="0"/>
         <v>6.7142857142857144</v>
       </c>
       <c r="J2">
-        <f>AVERAGE(J3:J51)</f>
+        <f t="shared" si="0"/>
         <v>153.11292546938779</v>
       </c>
     </row>
@@ -8132,8 +7684,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -8185,39 +7737,39 @@
         <v>62</v>
       </c>
       <c r="B2">
-        <f>AVERAGE(B3:B51)</f>
+        <f t="shared" ref="B2:J2" si="0">AVERAGE(B3:B51)</f>
         <v>639.16326530612241</v>
       </c>
       <c r="C2">
-        <f>AVERAGE(C3:C51)</f>
+        <f t="shared" si="0"/>
         <v>0.5714285714285714</v>
       </c>
       <c r="D2">
-        <f>AVERAGE(D3:D51)</f>
+        <f t="shared" si="0"/>
         <v>144.83624679591838</v>
       </c>
       <c r="E2">
-        <f>AVERAGE(E3:E51)</f>
+        <f t="shared" si="0"/>
         <v>147.36734693877551</v>
       </c>
       <c r="F2">
-        <f>AVERAGE(F3:F51)</f>
+        <f t="shared" si="0"/>
         <v>8.1632653061224483E-2</v>
       </c>
       <c r="G2">
-        <f>AVERAGE(G3:G51)</f>
+        <f t="shared" si="0"/>
         <v>187.3616095918367</v>
       </c>
       <c r="H2">
-        <f>AVERAGE(H3:H51)</f>
+        <f t="shared" si="0"/>
         <v>143.67346938775509</v>
       </c>
       <c r="I2">
-        <f>AVERAGE(I3:I51)</f>
+        <f t="shared" si="0"/>
         <v>0.14285714285714285</v>
       </c>
       <c r="J2">
-        <f>AVERAGE(J3:J51)</f>
+        <f t="shared" si="0"/>
         <v>189.73899469387752</v>
       </c>
     </row>
@@ -9819,6 +9371,1698 @@
       </c>
       <c r="J52">
         <v>104.66907999999999</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J52"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D23" sqref="D23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="10.28515625" customWidth="1"/>
+    <col min="2" max="6" width="14.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" t="s">
+        <v>4</v>
+      </c>
+      <c r="D1" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>7</v>
+      </c>
+      <c r="G1" t="s">
+        <v>8</v>
+      </c>
+      <c r="H1" t="s">
+        <v>9</v>
+      </c>
+      <c r="I1" t="s">
+        <v>10</v>
+      </c>
+      <c r="J1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2">
+        <f t="shared" ref="B2:J2" si="0">AVERAGE(B3:B51)</f>
+        <v>12177.65306122449</v>
+      </c>
+      <c r="C2">
+        <f t="shared" si="0"/>
+        <v>12.448979591836734</v>
+      </c>
+      <c r="D2">
+        <f t="shared" si="0"/>
+        <v>117.02324751020411</v>
+      </c>
+      <c r="E2">
+        <f t="shared" si="0"/>
+        <v>11984.714285714286</v>
+      </c>
+      <c r="F2">
+        <f t="shared" si="0"/>
+        <v>25.693877551020407</v>
+      </c>
+      <c r="G2">
+        <f t="shared" si="0"/>
+        <v>118.54178946938771</v>
+      </c>
+      <c r="H2">
+        <f t="shared" si="0"/>
+        <v>11779.408163265307</v>
+      </c>
+      <c r="I2">
+        <f t="shared" si="0"/>
+        <v>16.510204081632654</v>
+      </c>
+      <c r="J2">
+        <f t="shared" si="0"/>
+        <v>120.03179708163266</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B3">
+        <v>14214</v>
+      </c>
+      <c r="C3">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <v>136.5643</v>
+      </c>
+      <c r="E3">
+        <v>13825</v>
+      </c>
+      <c r="F3">
+        <v>15</v>
+      </c>
+      <c r="G3">
+        <v>136.5643</v>
+      </c>
+      <c r="H3">
+        <v>13285</v>
+      </c>
+      <c r="I3">
+        <v>13</v>
+      </c>
+      <c r="J3">
+        <v>136.5643</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>12</v>
+      </c>
+      <c r="B4">
+        <v>14604</v>
+      </c>
+      <c r="C4">
+        <v>13</v>
+      </c>
+      <c r="D4">
+        <v>129.40009000000001</v>
+      </c>
+      <c r="E4">
+        <v>14269</v>
+      </c>
+      <c r="F4">
+        <v>541</v>
+      </c>
+      <c r="G4">
+        <v>129.40009000000001</v>
+      </c>
+      <c r="H4">
+        <v>13806</v>
+      </c>
+      <c r="I4">
+        <v>11</v>
+      </c>
+      <c r="J4">
+        <v>129.40009000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5">
+        <v>13536</v>
+      </c>
+      <c r="C5">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>115.53062</v>
+      </c>
+      <c r="E5">
+        <v>13428</v>
+      </c>
+      <c r="F5">
+        <v>9</v>
+      </c>
+      <c r="G5">
+        <v>120.30083</v>
+      </c>
+      <c r="H5">
+        <v>13019</v>
+      </c>
+      <c r="I5">
+        <v>9</v>
+      </c>
+      <c r="J5">
+        <v>120.30083</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6">
+        <v>15643</v>
+      </c>
+      <c r="C6">
+        <v>10</v>
+      </c>
+      <c r="D6">
+        <v>156.38050000000001</v>
+      </c>
+      <c r="E6">
+        <v>15594</v>
+      </c>
+      <c r="F6">
+        <v>10</v>
+      </c>
+      <c r="G6">
+        <v>156.38050000000001</v>
+      </c>
+      <c r="H6">
+        <v>15515</v>
+      </c>
+      <c r="I6">
+        <v>11</v>
+      </c>
+      <c r="J6">
+        <v>156.38050000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>5580</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7">
+        <v>76.556359999999998</v>
+      </c>
+      <c r="E7">
+        <v>5477</v>
+      </c>
+      <c r="F7">
+        <v>3</v>
+      </c>
+      <c r="G7">
+        <v>76.556359999999998</v>
+      </c>
+      <c r="H7">
+        <v>5285</v>
+      </c>
+      <c r="I7">
+        <v>3</v>
+      </c>
+      <c r="J7">
+        <v>76.556359999999998</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B8">
+        <v>14390</v>
+      </c>
+      <c r="C8">
+        <v>9</v>
+      </c>
+      <c r="D8">
+        <v>137.67151000000001</v>
+      </c>
+      <c r="E8">
+        <v>14386</v>
+      </c>
+      <c r="F8">
+        <v>9</v>
+      </c>
+      <c r="G8">
+        <v>138.08573999999999</v>
+      </c>
+      <c r="H8">
+        <v>14257</v>
+      </c>
+      <c r="I8">
+        <v>10</v>
+      </c>
+      <c r="J8">
+        <v>138.08573999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>17</v>
+      </c>
+      <c r="B9">
+        <v>14239</v>
+      </c>
+      <c r="C9">
+        <v>9</v>
+      </c>
+      <c r="D9">
+        <v>136.24876</v>
+      </c>
+      <c r="E9">
+        <v>13740</v>
+      </c>
+      <c r="F9">
+        <v>10</v>
+      </c>
+      <c r="G9">
+        <v>136.24876</v>
+      </c>
+      <c r="H9">
+        <v>13352</v>
+      </c>
+      <c r="I9">
+        <v>9</v>
+      </c>
+      <c r="J9">
+        <v>136.24876</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10">
+        <v>14870</v>
+      </c>
+      <c r="C10">
+        <v>9</v>
+      </c>
+      <c r="D10">
+        <v>148.13538</v>
+      </c>
+      <c r="E10">
+        <v>14584</v>
+      </c>
+      <c r="F10">
+        <v>9</v>
+      </c>
+      <c r="G10">
+        <v>148.13538</v>
+      </c>
+      <c r="H10">
+        <v>14146</v>
+      </c>
+      <c r="I10">
+        <v>9</v>
+      </c>
+      <c r="J10">
+        <v>148.13538</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>19</v>
+      </c>
+      <c r="B11">
+        <v>15710</v>
+      </c>
+      <c r="C11">
+        <v>11</v>
+      </c>
+      <c r="D11">
+        <v>178.80206000000001</v>
+      </c>
+      <c r="E11">
+        <v>15678</v>
+      </c>
+      <c r="F11">
+        <v>13</v>
+      </c>
+      <c r="G11">
+        <v>178.80206000000001</v>
+      </c>
+      <c r="H11">
+        <v>15627</v>
+      </c>
+      <c r="I11">
+        <v>13</v>
+      </c>
+      <c r="J11">
+        <v>178.80206000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>63</v>
+      </c>
+      <c r="B12">
+        <v>14177</v>
+      </c>
+      <c r="C12">
+        <v>9</v>
+      </c>
+      <c r="D12">
+        <v>116.12376399999999</v>
+      </c>
+      <c r="E12">
+        <v>13998</v>
+      </c>
+      <c r="F12">
+        <v>9</v>
+      </c>
+      <c r="G12">
+        <v>118.5153</v>
+      </c>
+      <c r="H12">
+        <v>13648</v>
+      </c>
+      <c r="I12">
+        <v>9</v>
+      </c>
+      <c r="J12">
+        <v>118.5153</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13">
+        <v>15633</v>
+      </c>
+      <c r="C13">
+        <v>9</v>
+      </c>
+      <c r="D13">
+        <v>150.3664</v>
+      </c>
+      <c r="E13">
+        <v>15562</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
+      </c>
+      <c r="G13">
+        <v>155.01094000000001</v>
+      </c>
+      <c r="H13">
+        <v>15426</v>
+      </c>
+      <c r="I13">
+        <v>11</v>
+      </c>
+      <c r="J13">
+        <v>155.62860000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B14">
+        <v>15487</v>
+      </c>
+      <c r="C14">
+        <v>108</v>
+      </c>
+      <c r="D14">
+        <v>162.87009</v>
+      </c>
+      <c r="E14">
+        <v>15298</v>
+      </c>
+      <c r="F14">
+        <v>9</v>
+      </c>
+      <c r="G14">
+        <v>162.87009</v>
+      </c>
+      <c r="H14">
+        <v>15118</v>
+      </c>
+      <c r="I14">
+        <v>9</v>
+      </c>
+      <c r="J14">
+        <v>162.87009</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>22</v>
+      </c>
+      <c r="B15">
+        <v>5738</v>
+      </c>
+      <c r="C15">
+        <v>3</v>
+      </c>
+      <c r="D15">
+        <v>68.710160000000002</v>
+      </c>
+      <c r="E15">
+        <v>5935</v>
+      </c>
+      <c r="F15">
+        <v>3</v>
+      </c>
+      <c r="G15">
+        <v>72.445440000000005</v>
+      </c>
+      <c r="H15">
+        <v>6412</v>
+      </c>
+      <c r="I15">
+        <v>3</v>
+      </c>
+      <c r="J15">
+        <v>78.395195000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>23</v>
+      </c>
+      <c r="B16">
+        <v>15479</v>
+      </c>
+      <c r="C16">
+        <v>10</v>
+      </c>
+      <c r="D16">
+        <v>165.11578</v>
+      </c>
+      <c r="E16">
+        <v>15372</v>
+      </c>
+      <c r="F16">
+        <v>9</v>
+      </c>
+      <c r="G16">
+        <v>168.84616</v>
+      </c>
+      <c r="H16">
+        <v>15241</v>
+      </c>
+      <c r="I16">
+        <v>9</v>
+      </c>
+      <c r="J16">
+        <v>170.17458999999999</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>24</v>
+      </c>
+      <c r="B17">
+        <v>6543</v>
+      </c>
+      <c r="C17">
+        <v>4</v>
+      </c>
+      <c r="D17">
+        <v>74.913579999999996</v>
+      </c>
+      <c r="E17">
+        <v>6932</v>
+      </c>
+      <c r="F17">
+        <v>4</v>
+      </c>
+      <c r="G17">
+        <v>78.570440000000005</v>
+      </c>
+      <c r="H17">
+        <v>7543</v>
+      </c>
+      <c r="I17">
+        <v>4</v>
+      </c>
+      <c r="J17">
+        <v>84.145189999999999</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>25</v>
+      </c>
+      <c r="B18">
+        <v>13548</v>
+      </c>
+      <c r="C18">
+        <v>9</v>
+      </c>
+      <c r="D18">
+        <v>133.7886</v>
+      </c>
+      <c r="E18">
+        <v>12788</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+      <c r="G18">
+        <v>133.7886</v>
+      </c>
+      <c r="H18">
+        <v>12296</v>
+      </c>
+      <c r="I18">
+        <v>8</v>
+      </c>
+      <c r="J18">
+        <v>133.7886</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B19">
+        <v>8123</v>
+      </c>
+      <c r="C19">
+        <v>5</v>
+      </c>
+      <c r="D19">
+        <v>86.495699999999999</v>
+      </c>
+      <c r="E19">
+        <v>7806</v>
+      </c>
+      <c r="F19">
+        <v>5</v>
+      </c>
+      <c r="G19">
+        <v>91.449119999999994</v>
+      </c>
+      <c r="H19">
+        <v>7861</v>
+      </c>
+      <c r="I19">
+        <v>5</v>
+      </c>
+      <c r="J19">
+        <v>99.559399999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>27</v>
+      </c>
+      <c r="B20">
+        <v>13284</v>
+      </c>
+      <c r="C20">
+        <v>9</v>
+      </c>
+      <c r="D20">
+        <v>115.73344</v>
+      </c>
+      <c r="E20">
+        <v>13113</v>
+      </c>
+      <c r="F20">
+        <v>140</v>
+      </c>
+      <c r="G20">
+        <v>115.73344</v>
+      </c>
+      <c r="H20">
+        <v>12908</v>
+      </c>
+      <c r="I20">
+        <v>9</v>
+      </c>
+      <c r="J20">
+        <v>116.8903</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>28</v>
+      </c>
+      <c r="B21">
+        <v>6583</v>
+      </c>
+      <c r="C21">
+        <v>4</v>
+      </c>
+      <c r="D21">
+        <v>53.231605999999999</v>
+      </c>
+      <c r="E21">
+        <v>6966</v>
+      </c>
+      <c r="F21">
+        <v>5</v>
+      </c>
+      <c r="G21">
+        <v>56.888460000000002</v>
+      </c>
+      <c r="H21">
+        <v>7802</v>
+      </c>
+      <c r="I21">
+        <v>4</v>
+      </c>
+      <c r="J21">
+        <v>63.798996000000002</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>29</v>
+      </c>
+      <c r="B22">
+        <v>7058</v>
+      </c>
+      <c r="C22">
+        <v>4</v>
+      </c>
+      <c r="D22">
+        <v>59.724249999999998</v>
+      </c>
+      <c r="E22">
+        <v>7549</v>
+      </c>
+      <c r="F22">
+        <v>5</v>
+      </c>
+      <c r="G22">
+        <v>63.381104000000001</v>
+      </c>
+      <c r="H22">
+        <v>8024</v>
+      </c>
+      <c r="I22">
+        <v>4</v>
+      </c>
+      <c r="J22">
+        <v>66.863960000000006</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>30</v>
+      </c>
+      <c r="B23">
+        <v>10462</v>
+      </c>
+      <c r="C23">
+        <v>6</v>
+      </c>
+      <c r="D23">
+        <v>123.20586</v>
+      </c>
+      <c r="E23">
+        <v>10137</v>
+      </c>
+      <c r="F23">
+        <v>7</v>
+      </c>
+      <c r="G23">
+        <v>123.20586</v>
+      </c>
+      <c r="H23">
+        <v>9929</v>
+      </c>
+      <c r="I23">
+        <v>6</v>
+      </c>
+      <c r="J23">
+        <v>123.20586</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24">
+        <v>12712</v>
+      </c>
+      <c r="C24">
+        <v>9</v>
+      </c>
+      <c r="D24">
+        <v>111.91296</v>
+      </c>
+      <c r="E24">
+        <v>12297</v>
+      </c>
+      <c r="F24">
+        <v>8</v>
+      </c>
+      <c r="G24">
+        <v>111.91296</v>
+      </c>
+      <c r="H24">
+        <v>12009</v>
+      </c>
+      <c r="I24">
+        <v>9</v>
+      </c>
+      <c r="J24">
+        <v>111.91296</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25">
+        <v>10390</v>
+      </c>
+      <c r="C25">
+        <v>7</v>
+      </c>
+      <c r="D25">
+        <v>93.545950000000005</v>
+      </c>
+      <c r="E25">
+        <v>9950</v>
+      </c>
+      <c r="F25">
+        <v>7</v>
+      </c>
+      <c r="G25">
+        <v>93.545950000000005</v>
+      </c>
+      <c r="H25">
+        <v>9612</v>
+      </c>
+      <c r="I25">
+        <v>6</v>
+      </c>
+      <c r="J25">
+        <v>93.545950000000005</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>33</v>
+      </c>
+      <c r="B26">
+        <v>14235</v>
+      </c>
+      <c r="C26">
+        <v>13</v>
+      </c>
+      <c r="D26">
+        <v>126.62743</v>
+      </c>
+      <c r="E26">
+        <v>13987</v>
+      </c>
+      <c r="F26">
+        <v>12</v>
+      </c>
+      <c r="G26">
+        <v>126.62743</v>
+      </c>
+      <c r="H26">
+        <v>13725</v>
+      </c>
+      <c r="I26">
+        <v>299</v>
+      </c>
+      <c r="J26">
+        <v>126.62743</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>34</v>
+      </c>
+      <c r="B27">
+        <v>9017</v>
+      </c>
+      <c r="C27">
+        <v>6</v>
+      </c>
+      <c r="D27">
+        <v>91.545944000000006</v>
+      </c>
+      <c r="E27">
+        <v>8358</v>
+      </c>
+      <c r="F27">
+        <v>6</v>
+      </c>
+      <c r="G27">
+        <v>91.545944000000006</v>
+      </c>
+      <c r="H27">
+        <v>7695</v>
+      </c>
+      <c r="I27">
+        <v>5</v>
+      </c>
+      <c r="J27">
+        <v>91.545944000000006</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28">
+        <v>8120</v>
+      </c>
+      <c r="C28">
+        <v>5</v>
+      </c>
+      <c r="D28">
+        <v>88.045944000000006</v>
+      </c>
+      <c r="E28">
+        <v>7404</v>
+      </c>
+      <c r="F28">
+        <v>4</v>
+      </c>
+      <c r="G28">
+        <v>88.045944000000006</v>
+      </c>
+      <c r="H28">
+        <v>6822</v>
+      </c>
+      <c r="I28">
+        <v>5</v>
+      </c>
+      <c r="J28">
+        <v>88.045944000000006</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>36</v>
+      </c>
+      <c r="B29">
+        <v>9992</v>
+      </c>
+      <c r="C29">
+        <v>6</v>
+      </c>
+      <c r="D29">
+        <v>118.38479</v>
+      </c>
+      <c r="E29">
+        <v>9588</v>
+      </c>
+      <c r="F29">
+        <v>189</v>
+      </c>
+      <c r="G29">
+        <v>118.38479</v>
+      </c>
+      <c r="H29">
+        <v>9300</v>
+      </c>
+      <c r="I29">
+        <v>6</v>
+      </c>
+      <c r="J29">
+        <v>118.38479</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>37</v>
+      </c>
+      <c r="B30">
+        <v>9554</v>
+      </c>
+      <c r="C30">
+        <v>11</v>
+      </c>
+      <c r="D30">
+        <v>86.441149999999993</v>
+      </c>
+      <c r="E30">
+        <v>9146</v>
+      </c>
+      <c r="F30">
+        <v>12</v>
+      </c>
+      <c r="G30">
+        <v>86.441149999999993</v>
+      </c>
+      <c r="H30">
+        <v>8761</v>
+      </c>
+      <c r="I30">
+        <v>9</v>
+      </c>
+      <c r="J30">
+        <v>86.441149999999993</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>38</v>
+      </c>
+      <c r="B31">
+        <v>10198</v>
+      </c>
+      <c r="C31">
+        <v>6</v>
+      </c>
+      <c r="D31">
+        <v>125.127426</v>
+      </c>
+      <c r="E31">
+        <v>9784</v>
+      </c>
+      <c r="F31">
+        <v>9</v>
+      </c>
+      <c r="G31">
+        <v>125.127426</v>
+      </c>
+      <c r="H31">
+        <v>9473</v>
+      </c>
+      <c r="I31">
+        <v>6</v>
+      </c>
+      <c r="J31">
+        <v>125.127426</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>39</v>
+      </c>
+      <c r="B32">
+        <v>11718</v>
+      </c>
+      <c r="C32">
+        <v>13</v>
+      </c>
+      <c r="D32">
+        <v>101.19113</v>
+      </c>
+      <c r="E32">
+        <v>11192</v>
+      </c>
+      <c r="F32">
+        <v>11</v>
+      </c>
+      <c r="G32">
+        <v>101.19113</v>
+      </c>
+      <c r="H32">
+        <v>10770</v>
+      </c>
+      <c r="I32">
+        <v>13</v>
+      </c>
+      <c r="J32">
+        <v>101.19113</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>40</v>
+      </c>
+      <c r="B33">
+        <v>8478</v>
+      </c>
+      <c r="C33">
+        <v>6</v>
+      </c>
+      <c r="D33">
+        <v>96.322599999999994</v>
+      </c>
+      <c r="E33">
+        <v>8112</v>
+      </c>
+      <c r="F33">
+        <v>5</v>
+      </c>
+      <c r="G33">
+        <v>96.322599999999994</v>
+      </c>
+      <c r="H33">
+        <v>7749</v>
+      </c>
+      <c r="I33">
+        <v>6</v>
+      </c>
+      <c r="J33">
+        <v>96.322599999999994</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>41</v>
+      </c>
+      <c r="B34">
+        <v>14380</v>
+      </c>
+      <c r="C34">
+        <v>13</v>
+      </c>
+      <c r="D34">
+        <v>119.948494</v>
+      </c>
+      <c r="E34">
+        <v>14415</v>
+      </c>
+      <c r="F34">
+        <v>14</v>
+      </c>
+      <c r="G34">
+        <v>127.058784</v>
+      </c>
+      <c r="H34">
+        <v>14453</v>
+      </c>
+      <c r="I34">
+        <v>14</v>
+      </c>
+      <c r="J34">
+        <v>134.91539</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>42</v>
+      </c>
+      <c r="B35">
+        <v>15727</v>
+      </c>
+      <c r="C35">
+        <v>14</v>
+      </c>
+      <c r="D35">
+        <v>183.05538999999999</v>
+      </c>
+      <c r="E35">
+        <v>15684</v>
+      </c>
+      <c r="F35">
+        <v>11</v>
+      </c>
+      <c r="G35">
+        <v>183.05538999999999</v>
+      </c>
+      <c r="H35">
+        <v>15615</v>
+      </c>
+      <c r="I35">
+        <v>15</v>
+      </c>
+      <c r="J35">
+        <v>183.38381999999999</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36">
+        <v>8470</v>
+      </c>
+      <c r="C36">
+        <v>7</v>
+      </c>
+      <c r="D36">
+        <v>97.943923999999996</v>
+      </c>
+      <c r="E36">
+        <v>8102</v>
+      </c>
+      <c r="F36">
+        <v>7</v>
+      </c>
+      <c r="G36">
+        <v>97.943923999999996</v>
+      </c>
+      <c r="H36">
+        <v>7731</v>
+      </c>
+      <c r="I36">
+        <v>10</v>
+      </c>
+      <c r="J36">
+        <v>97.943923999999996</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>44</v>
+      </c>
+      <c r="B37">
+        <v>7363</v>
+      </c>
+      <c r="C37">
+        <v>6</v>
+      </c>
+      <c r="D37">
+        <v>107.95586400000001</v>
+      </c>
+      <c r="E37">
+        <v>6908</v>
+      </c>
+      <c r="F37">
+        <v>7</v>
+      </c>
+      <c r="G37">
+        <v>107.95586400000001</v>
+      </c>
+      <c r="H37">
+        <v>6591</v>
+      </c>
+      <c r="I37">
+        <v>5</v>
+      </c>
+      <c r="J37">
+        <v>107.95586400000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>45</v>
+      </c>
+      <c r="B38">
+        <v>15693</v>
+      </c>
+      <c r="C38">
+        <v>10</v>
+      </c>
+      <c r="D38">
+        <v>164.22695999999999</v>
+      </c>
+      <c r="E38">
+        <v>15634</v>
+      </c>
+      <c r="F38">
+        <v>11</v>
+      </c>
+      <c r="G38">
+        <v>164.22695999999999</v>
+      </c>
+      <c r="H38">
+        <v>15554</v>
+      </c>
+      <c r="I38">
+        <v>11</v>
+      </c>
+      <c r="J38">
+        <v>164.55538999999999</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
+        <v>46</v>
+      </c>
+      <c r="B39">
+        <v>14345</v>
+      </c>
+      <c r="C39">
+        <v>9</v>
+      </c>
+      <c r="D39">
+        <v>110.62006</v>
+      </c>
+      <c r="E39">
+        <v>14431</v>
+      </c>
+      <c r="F39">
+        <v>10</v>
+      </c>
+      <c r="G39">
+        <v>117.73035400000001</v>
+      </c>
+      <c r="H39">
+        <v>14500</v>
+      </c>
+      <c r="I39">
+        <v>11</v>
+      </c>
+      <c r="J39">
+        <v>125.58696</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40">
+        <v>13355</v>
+      </c>
+      <c r="C40">
+        <v>10</v>
+      </c>
+      <c r="D40">
+        <v>109.36548999999999</v>
+      </c>
+      <c r="E40">
+        <v>12340</v>
+      </c>
+      <c r="F40">
+        <v>8</v>
+      </c>
+      <c r="G40">
+        <v>109.36548999999999</v>
+      </c>
+      <c r="H40">
+        <v>11369</v>
+      </c>
+      <c r="I40">
+        <v>9</v>
+      </c>
+      <c r="J40">
+        <v>109.36548999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>48</v>
+      </c>
+      <c r="B41">
+        <v>13542</v>
+      </c>
+      <c r="C41">
+        <v>9</v>
+      </c>
+      <c r="D41">
+        <v>110.10903999999999</v>
+      </c>
+      <c r="E41">
+        <v>14419</v>
+      </c>
+      <c r="F41">
+        <v>9</v>
+      </c>
+      <c r="G41">
+        <v>123.26957</v>
+      </c>
+      <c r="H41">
+        <v>14550</v>
+      </c>
+      <c r="I41">
+        <v>11</v>
+      </c>
+      <c r="J41">
+        <v>130.99446</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>49</v>
+      </c>
+      <c r="B42">
+        <v>15727</v>
+      </c>
+      <c r="C42">
+        <v>10</v>
+      </c>
+      <c r="D42">
+        <v>164.6412</v>
+      </c>
+      <c r="E42">
+        <v>15670</v>
+      </c>
+      <c r="F42">
+        <v>11</v>
+      </c>
+      <c r="G42">
+        <v>164.80542</v>
+      </c>
+      <c r="H42">
+        <v>15584</v>
+      </c>
+      <c r="I42">
+        <v>10</v>
+      </c>
+      <c r="J42">
+        <v>165.46227999999999</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43">
+        <v>14980</v>
+      </c>
+      <c r="C43">
+        <v>10</v>
+      </c>
+      <c r="D43">
+        <v>117.98833999999999</v>
+      </c>
+      <c r="E43">
+        <v>14851</v>
+      </c>
+      <c r="F43">
+        <v>10</v>
+      </c>
+      <c r="G43">
+        <v>121.02388000000001</v>
+      </c>
+      <c r="H43">
+        <v>14993</v>
+      </c>
+      <c r="I43">
+        <v>10</v>
+      </c>
+      <c r="J43">
+        <v>128.97210000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>51</v>
+      </c>
+      <c r="B44">
+        <v>14023</v>
+      </c>
+      <c r="C44">
+        <v>66</v>
+      </c>
+      <c r="D44">
+        <v>123.150406</v>
+      </c>
+      <c r="E44">
+        <v>13750</v>
+      </c>
+      <c r="F44">
+        <v>8</v>
+      </c>
+      <c r="G44">
+        <v>123.150406</v>
+      </c>
+      <c r="H44">
+        <v>13709</v>
+      </c>
+      <c r="I44">
+        <v>9</v>
+      </c>
+      <c r="J44">
+        <v>124.79255999999999</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>52</v>
+      </c>
+      <c r="B45">
+        <v>14932</v>
+      </c>
+      <c r="C45">
+        <v>10</v>
+      </c>
+      <c r="D45">
+        <v>116.18226</v>
+      </c>
+      <c r="E45">
+        <v>14517</v>
+      </c>
+      <c r="F45">
+        <v>9</v>
+      </c>
+      <c r="G45">
+        <v>116.18226</v>
+      </c>
+      <c r="H45">
+        <v>14178</v>
+      </c>
+      <c r="I45">
+        <v>9</v>
+      </c>
+      <c r="J45">
+        <v>116.34647</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>53</v>
+      </c>
+      <c r="B46">
+        <v>8241</v>
+      </c>
+      <c r="C46">
+        <v>5</v>
+      </c>
+      <c r="D46">
+        <v>81.069810000000004</v>
+      </c>
+      <c r="E46">
+        <v>7887</v>
+      </c>
+      <c r="F46">
+        <v>4</v>
+      </c>
+      <c r="G46">
+        <v>81.069810000000004</v>
+      </c>
+      <c r="H46">
+        <v>7512</v>
+      </c>
+      <c r="I46">
+        <v>5</v>
+      </c>
+      <c r="J46">
+        <v>81.069810000000004</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>54</v>
+      </c>
+      <c r="B47">
+        <v>14898</v>
+      </c>
+      <c r="C47">
+        <v>9</v>
+      </c>
+      <c r="D47">
+        <v>122.534294</v>
+      </c>
+      <c r="E47">
+        <v>14621</v>
+      </c>
+      <c r="F47">
+        <v>10</v>
+      </c>
+      <c r="G47">
+        <v>122.534294</v>
+      </c>
+      <c r="H47">
+        <v>12710</v>
+      </c>
+      <c r="I47">
+        <v>114</v>
+      </c>
+      <c r="J47">
+        <v>122.534294</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>55</v>
+      </c>
+      <c r="B48">
+        <v>15606</v>
+      </c>
+      <c r="C48">
+        <v>10</v>
+      </c>
+      <c r="D48">
+        <v>137.98708999999999</v>
+      </c>
+      <c r="E48">
+        <v>15268</v>
+      </c>
+      <c r="F48">
+        <v>10</v>
+      </c>
+      <c r="G48">
+        <v>137.98708999999999</v>
+      </c>
+      <c r="H48">
+        <v>15013</v>
+      </c>
+      <c r="I48">
+        <v>9</v>
+      </c>
+      <c r="J48">
+        <v>137.98708999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>56</v>
+      </c>
+      <c r="B49">
+        <v>15564</v>
+      </c>
+      <c r="C49">
+        <v>12</v>
+      </c>
+      <c r="D49">
+        <v>135.40129999999999</v>
+      </c>
+      <c r="E49">
+        <v>15477</v>
+      </c>
+      <c r="F49">
+        <v>10</v>
+      </c>
+      <c r="G49">
+        <v>135.40129999999999</v>
+      </c>
+      <c r="H49">
+        <v>15047</v>
+      </c>
+      <c r="I49">
+        <v>10</v>
+      </c>
+      <c r="J49">
+        <v>135.40129999999999</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>57</v>
+      </c>
+      <c r="B50">
+        <v>5273</v>
+      </c>
+      <c r="C50">
+        <v>4</v>
+      </c>
+      <c r="D50">
+        <v>52.923096000000001</v>
+      </c>
+      <c r="E50">
+        <v>6058</v>
+      </c>
+      <c r="F50">
+        <v>4</v>
+      </c>
+      <c r="G50">
+        <v>61.101399999999998</v>
+      </c>
+      <c r="H50">
+        <v>7111</v>
+      </c>
+      <c r="I50">
+        <v>4</v>
+      </c>
+      <c r="J50">
+        <v>66.474239999999995</v>
+      </c>
+    </row>
+    <row r="51" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>58</v>
+      </c>
+      <c r="B51">
+        <v>15271</v>
+      </c>
+      <c r="C51">
+        <v>10</v>
+      </c>
+      <c r="D51">
+        <v>114.32197600000001</v>
+      </c>
+      <c r="E51">
+        <v>14964</v>
+      </c>
+      <c r="F51">
+        <v>10</v>
+      </c>
+      <c r="G51">
+        <v>114.36118999999999</v>
+      </c>
+      <c r="H51">
+        <v>14555</v>
+      </c>
+      <c r="I51">
+        <v>10</v>
+      </c>
+      <c r="J51">
+        <v>114.36118999999999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>59</v>
+      </c>
+      <c r="B52">
+        <v>6704</v>
+      </c>
+      <c r="C52">
+        <v>4</v>
+      </c>
+      <c r="D52">
+        <v>56.584519999999998</v>
+      </c>
+      <c r="E52">
+        <v>6352</v>
+      </c>
+      <c r="F52">
+        <v>4</v>
+      </c>
+      <c r="G52">
+        <v>56.584519999999998</v>
+      </c>
+      <c r="H52">
+        <v>5900</v>
+      </c>
+      <c r="I52">
+        <v>4</v>
+      </c>
+      <c r="J52">
+        <v>56.584519999999998</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Project 1 is all done besides Integrated A*
</commit_message>
<xml_diff>
--- a/Documents/Project 1 search averages.xlsx
+++ b/Documents/Project 1 search averages.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12795"/>
   </bookViews>
   <sheets>
     <sheet name="Final Averages" sheetId="13" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="92">
   <si>
     <t>UCS nodes</t>
   </si>
@@ -284,13 +284,28 @@
     <t>Time in MS</t>
   </si>
   <si>
-    <t>1.25 weight A* cost</t>
+    <t>2 weight Sequential A*</t>
   </si>
   <si>
-    <t>1.25 weight A* time</t>
+    <t>1.25 weight Sequential A*</t>
   </si>
   <si>
-    <t>1.25 weight A* nodes</t>
+    <t>1.25 weight Sequential A* nodes</t>
+  </si>
+  <si>
+    <t>1.25 weight Sequential A* time</t>
+  </si>
+  <si>
+    <t>1.25 weight Sequential A* cost</t>
+  </si>
+  <si>
+    <t>2 weight Sequential A* nodes</t>
+  </si>
+  <si>
+    <t>2 weight Sequential A* time</t>
+  </si>
+  <si>
+    <t>2 weight Sequential A* cost</t>
   </si>
 </sst>
 </file>
@@ -645,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D17"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -903,6 +918,34 @@
         <v>189.73899469387752</v>
       </c>
     </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B18" s="1">
+        <v>8907.5510204081638</v>
+      </c>
+      <c r="C18" s="1">
+        <v>37.122448979591837</v>
+      </c>
+      <c r="D18" s="1">
+        <v>113.37456379591833</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B19" s="1">
+        <v>6968.7142857142853</v>
+      </c>
+      <c r="C19" s="1">
+        <v>55.469387755101998</v>
+      </c>
+      <c r="D19" s="1">
+        <v>114.05043887755102</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -912,19 +955,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:G1048576"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="29" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="28.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="46" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="46" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
@@ -935,19 +980,19 @@
         <v>86</v>
       </c>
       <c r="C1" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="D1" t="s">
-        <v>84</v>
+        <v>88</v>
       </c>
       <c r="E1" t="s">
-        <v>6</v>
+        <v>89</v>
       </c>
       <c r="F1" t="s">
-        <v>7</v>
+        <v>90</v>
       </c>
       <c r="G1" t="s">
-        <v>8</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -956,27 +1001,27 @@
       </c>
       <c r="B2">
         <f t="shared" ref="B2:G2" si="0">AVERAGE(B3:B51)</f>
-        <v>11945.612244897959</v>
+        <v>8907.5510204081638</v>
       </c>
       <c r="C2">
         <f t="shared" si="0"/>
-        <v>118.44897959183673</v>
+        <v>37.122448979591837</v>
       </c>
       <c r="D2">
         <f t="shared" si="0"/>
-        <v>113.42658430612244</v>
+        <v>113.37456379591833</v>
       </c>
       <c r="E2">
         <f t="shared" si="0"/>
-        <v>11221.693877551021</v>
+        <v>6968.7142857142853</v>
       </c>
       <c r="F2">
         <f t="shared" si="0"/>
-        <v>111</v>
+        <v>55.469387755102041</v>
       </c>
       <c r="G2">
         <f t="shared" si="0"/>
-        <v>113.88519681632653</v>
+        <v>114.05043887755102</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -987,7 +1032,7 @@
         <v>10212</v>
       </c>
       <c r="C3">
-        <v>405</v>
+        <v>60</v>
       </c>
       <c r="D3">
         <v>136.5643</v>
@@ -996,7 +1041,7 @@
         <v>6822</v>
       </c>
       <c r="F3">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G3">
         <v>136.5643</v>
@@ -1007,19 +1052,19 @@
         <v>12</v>
       </c>
       <c r="B4">
-        <v>11870</v>
+        <v>10652</v>
       </c>
       <c r="C4">
-        <v>32</v>
+        <v>531</v>
       </c>
       <c r="D4">
         <v>129.40009000000001</v>
       </c>
       <c r="E4">
-        <v>6883</v>
+        <v>7448</v>
       </c>
       <c r="F4">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="G4">
         <v>129.40009000000001</v>
@@ -1030,19 +1075,19 @@
         <v>13</v>
       </c>
       <c r="B5">
-        <v>9984</v>
+        <v>9844</v>
       </c>
       <c r="C5">
-        <v>18</v>
+        <v>22</v>
       </c>
       <c r="D5">
         <v>115.53062</v>
       </c>
       <c r="E5">
-        <v>6972</v>
+        <v>8633</v>
       </c>
       <c r="F5">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G5">
         <v>115.53062</v>
@@ -1053,22 +1098,22 @@
         <v>14</v>
       </c>
       <c r="B6">
-        <v>15636</v>
+        <v>15096</v>
       </c>
       <c r="C6">
-        <v>88</v>
+        <v>69</v>
       </c>
       <c r="D6">
         <v>156.55205000000001</v>
       </c>
       <c r="E6">
-        <v>15433</v>
+        <v>12815</v>
       </c>
       <c r="F6">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="G6">
-        <v>156.55205000000001</v>
+        <v>157.04470000000001</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1076,7 +1121,7 @@
         <v>15</v>
       </c>
       <c r="B7">
-        <v>3145</v>
+        <v>2521</v>
       </c>
       <c r="C7">
         <v>4</v>
@@ -1085,7 +1130,7 @@
         <v>76.556359999999998</v>
       </c>
       <c r="E7">
-        <v>2263</v>
+        <v>2127</v>
       </c>
       <c r="F7">
         <v>3</v>
@@ -1099,19 +1144,19 @@
         <v>16</v>
       </c>
       <c r="B8">
-        <v>15487</v>
+        <v>9004</v>
       </c>
       <c r="C8">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="D8">
         <v>135.94968</v>
       </c>
       <c r="E8">
-        <v>15638</v>
+        <v>7125</v>
       </c>
       <c r="F8">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="G8">
         <v>135.94968</v>
@@ -1122,19 +1167,19 @@
         <v>17</v>
       </c>
       <c r="B9">
-        <v>9746</v>
+        <v>9076</v>
       </c>
       <c r="C9">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D9">
         <v>136.24876</v>
       </c>
       <c r="E9">
-        <v>6965</v>
+        <v>6733</v>
       </c>
       <c r="F9">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="G9">
         <v>136.24876</v>
@@ -1145,19 +1190,19 @@
         <v>18</v>
       </c>
       <c r="B10">
-        <v>12390</v>
+        <v>11226</v>
       </c>
       <c r="C10">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D10">
         <v>148.29958999999999</v>
       </c>
       <c r="E10">
-        <v>8376</v>
+        <v>7650</v>
       </c>
       <c r="F10">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G10">
         <v>148.29958999999999</v>
@@ -1168,22 +1213,22 @@
         <v>19</v>
       </c>
       <c r="B11">
-        <v>15720</v>
+        <v>15558</v>
       </c>
       <c r="C11">
-        <v>92</v>
+        <v>33</v>
       </c>
       <c r="D11">
         <v>178.80206000000001</v>
       </c>
       <c r="E11">
-        <v>15696</v>
+        <v>13515</v>
       </c>
       <c r="F11">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="G11">
-        <v>178.80206000000001</v>
+        <v>179.29471000000001</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
@@ -1191,19 +1236,19 @@
         <v>63</v>
       </c>
       <c r="B12">
-        <v>12118</v>
+        <v>11787</v>
       </c>
       <c r="C12">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D12">
         <v>116.12376399999999</v>
       </c>
       <c r="E12">
-        <v>8914</v>
+        <v>8777</v>
       </c>
       <c r="F12">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="G12">
         <v>116.12376399999999</v>
@@ -1214,22 +1259,22 @@
         <v>20</v>
       </c>
       <c r="B13">
-        <v>15707</v>
+        <v>15044</v>
       </c>
       <c r="C13">
-        <v>104</v>
+        <v>26</v>
       </c>
       <c r="D13">
         <v>141.29163</v>
       </c>
       <c r="E13">
-        <v>15692</v>
+        <v>13252</v>
       </c>
       <c r="F13">
-        <v>261</v>
+        <v>23</v>
       </c>
       <c r="G13">
-        <v>141.29163</v>
+        <v>141.94848999999999</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1237,22 +1282,22 @@
         <v>21</v>
       </c>
       <c r="B14">
-        <v>15666</v>
+        <v>14852</v>
       </c>
       <c r="C14">
-        <v>71</v>
+        <v>26</v>
       </c>
       <c r="D14">
         <v>151.76651000000001</v>
       </c>
       <c r="E14">
-        <v>15671</v>
+        <v>12506</v>
       </c>
       <c r="F14">
-        <v>72</v>
+        <v>22</v>
       </c>
       <c r="G14">
-        <v>152.2518</v>
+        <v>151.76651000000001</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1260,19 +1305,19 @@
         <v>22</v>
       </c>
       <c r="B15">
-        <v>3093</v>
+        <v>2861</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D15">
         <v>52.931980000000003</v>
       </c>
       <c r="E15">
-        <v>2266</v>
+        <v>1220</v>
       </c>
       <c r="F15">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G15">
         <v>53.096195000000002</v>
@@ -1283,19 +1328,19 @@
         <v>23</v>
       </c>
       <c r="B16">
-        <v>14548</v>
+        <v>14046</v>
       </c>
       <c r="C16">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="D16">
         <v>153.33760000000001</v>
       </c>
       <c r="E16">
-        <v>12480</v>
+        <v>11064</v>
       </c>
       <c r="F16">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="G16">
         <v>153.33760000000001</v>
@@ -1306,22 +1351,22 @@
         <v>24</v>
       </c>
       <c r="B17">
-        <v>5503</v>
+        <v>1617</v>
       </c>
       <c r="C17">
-        <v>16</v>
+        <v>2</v>
       </c>
       <c r="D17">
-        <v>59.174619999999997</v>
+        <v>58.846195000000002</v>
       </c>
       <c r="E17">
-        <v>5138</v>
+        <v>691</v>
       </c>
       <c r="F17">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="G17">
-        <v>59.174619999999997</v>
+        <v>58.846195000000002</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1329,22 +1374,22 @@
         <v>25</v>
       </c>
       <c r="B18">
-        <v>14544</v>
+        <v>9545</v>
       </c>
       <c r="C18">
-        <v>213</v>
+        <v>173</v>
       </c>
       <c r="D18">
         <v>123.65992</v>
       </c>
       <c r="E18">
-        <v>14557</v>
+        <v>7028</v>
       </c>
       <c r="F18">
-        <v>81</v>
+        <v>14</v>
       </c>
       <c r="G18">
-        <v>124.14521000000001</v>
+        <v>123.65992</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
@@ -1352,22 +1397,22 @@
         <v>26</v>
       </c>
       <c r="B19">
-        <v>12919</v>
+        <v>3452</v>
       </c>
       <c r="C19">
-        <v>25</v>
+        <v>4</v>
       </c>
       <c r="D19">
-        <v>74.881739999999994</v>
+        <v>74.717519999999993</v>
       </c>
       <c r="E19">
-        <v>14385</v>
+        <v>1780</v>
       </c>
       <c r="F19">
-        <v>28</v>
+        <v>2</v>
       </c>
       <c r="G19">
-        <v>74.881739999999994</v>
+        <v>76.852320000000006</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
@@ -1375,22 +1420,22 @@
         <v>27</v>
       </c>
       <c r="B20">
-        <v>10719</v>
+        <v>10473</v>
       </c>
       <c r="C20">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D20">
         <v>107.22363</v>
       </c>
       <c r="E20">
-        <v>7488</v>
+        <v>7945</v>
       </c>
       <c r="F20">
         <v>11</v>
       </c>
       <c r="G20">
-        <v>107.22363</v>
+        <v>107.534294</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
@@ -1398,22 +1443,22 @@
         <v>28</v>
       </c>
       <c r="B21">
-        <v>5622</v>
+        <v>900</v>
       </c>
       <c r="C21">
-        <v>16</v>
+        <v>1</v>
       </c>
       <c r="D21">
         <v>37.164214999999999</v>
       </c>
       <c r="E21">
-        <v>5299</v>
+        <v>375</v>
       </c>
       <c r="F21">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="G21">
-        <v>37.164214999999999</v>
+        <v>37.656860000000002</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
@@ -1421,22 +1466,22 @@
         <v>29</v>
       </c>
       <c r="B22">
-        <v>5840</v>
+        <v>1633</v>
       </c>
       <c r="C22">
-        <v>15</v>
+        <v>1</v>
       </c>
       <c r="D22">
-        <v>44.235287</v>
+        <v>43.656860000000002</v>
       </c>
       <c r="E22">
-        <v>5637</v>
+        <v>2361</v>
       </c>
       <c r="F22">
-        <v>17</v>
+        <v>3</v>
       </c>
       <c r="G22">
-        <v>43.656860000000002</v>
+        <v>54.798996000000002</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
@@ -1444,16 +1489,16 @@
         <v>30</v>
       </c>
       <c r="B23">
-        <v>7527</v>
+        <v>7318</v>
       </c>
       <c r="C23">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D23">
         <v>123.412964</v>
       </c>
       <c r="E23">
-        <v>6290</v>
+        <v>5843</v>
       </c>
       <c r="F23">
         <v>8</v>
@@ -1467,16 +1512,16 @@
         <v>31</v>
       </c>
       <c r="B24">
-        <v>10171</v>
+        <v>9755</v>
       </c>
       <c r="C24">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D24">
         <v>112.07717</v>
       </c>
       <c r="E24">
-        <v>7147</v>
+        <v>6458</v>
       </c>
       <c r="F24">
         <v>9</v>
@@ -1490,22 +1535,22 @@
         <v>32</v>
       </c>
       <c r="B25">
-        <v>14498</v>
+        <v>5091</v>
       </c>
       <c r="C25">
-        <v>30</v>
+        <v>6</v>
       </c>
       <c r="D25">
-        <v>94.038589999999999</v>
+        <v>93.545944000000006</v>
       </c>
       <c r="E25">
-        <v>15243</v>
+        <v>3844</v>
       </c>
       <c r="F25">
-        <v>35</v>
+        <v>5</v>
       </c>
       <c r="G25">
-        <v>95.634789999999995</v>
+        <v>93.545944000000006</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
@@ -1513,22 +1558,22 @@
         <v>33</v>
       </c>
       <c r="B26">
-        <v>13588</v>
+        <v>10303</v>
       </c>
       <c r="C26">
-        <v>287</v>
+        <v>16</v>
       </c>
       <c r="D26">
         <v>126.56553</v>
       </c>
       <c r="E26">
-        <v>13210</v>
+        <v>7447</v>
       </c>
       <c r="F26">
-        <v>59</v>
+        <v>11</v>
       </c>
       <c r="G26">
-        <v>126.56553</v>
+        <v>126.83454</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -1536,22 +1581,22 @@
         <v>34</v>
       </c>
       <c r="B27">
-        <v>14103</v>
+        <v>6162</v>
       </c>
       <c r="C27">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="D27">
-        <v>91.710160000000002</v>
+        <v>91.545944000000006</v>
       </c>
       <c r="E27">
-        <v>14730</v>
+        <v>4881</v>
       </c>
       <c r="F27">
-        <v>26</v>
+        <v>6</v>
       </c>
       <c r="G27">
-        <v>92.867019999999997</v>
+        <v>92.038589999999999</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
@@ -1559,22 +1604,22 @@
         <v>35</v>
       </c>
       <c r="B28">
-        <v>13692</v>
+        <v>5667</v>
       </c>
       <c r="C28">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="D28">
-        <v>88.417270000000002</v>
+        <v>88.253050000000002</v>
       </c>
       <c r="E28">
-        <v>14450</v>
+        <v>4497</v>
       </c>
       <c r="F28">
-        <v>182</v>
+        <v>6</v>
       </c>
       <c r="G28">
-        <v>89.574129999999997</v>
+        <v>88.909903999999997</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
@@ -1582,7 +1627,7 @@
         <v>36</v>
       </c>
       <c r="B29">
-        <v>7367</v>
+        <v>7288</v>
       </c>
       <c r="C29">
         <v>10</v>
@@ -1591,13 +1636,13 @@
         <v>118.38479</v>
       </c>
       <c r="E29">
-        <v>6075</v>
+        <v>5897</v>
       </c>
       <c r="F29">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G29">
-        <v>119.21322000000001</v>
+        <v>118.38479</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
@@ -1605,22 +1650,22 @@
         <v>37</v>
       </c>
       <c r="B30">
-        <v>11686</v>
+        <v>4764</v>
       </c>
       <c r="C30">
-        <v>41</v>
+        <v>246</v>
       </c>
       <c r="D30">
         <v>86.441153999999997</v>
       </c>
       <c r="E30">
-        <v>11367</v>
+        <v>2311</v>
       </c>
       <c r="F30">
-        <v>48</v>
+        <v>2</v>
       </c>
       <c r="G30">
-        <v>89.161709999999999</v>
+        <v>86.441153999999997</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
@@ -1628,19 +1673,19 @@
         <v>38</v>
       </c>
       <c r="B31">
-        <v>7256</v>
+        <v>7022</v>
       </c>
       <c r="C31">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D31">
         <v>125.127426</v>
       </c>
       <c r="E31">
-        <v>5879</v>
+        <v>5457</v>
       </c>
       <c r="F31">
-        <v>204</v>
+        <v>7</v>
       </c>
       <c r="G31">
         <v>125.127426</v>
@@ -1651,19 +1696,19 @@
         <v>39</v>
       </c>
       <c r="B32">
-        <v>7857</v>
+        <v>7272</v>
       </c>
       <c r="C32">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D32">
         <v>101.19113</v>
       </c>
       <c r="E32">
-        <v>6002</v>
+        <v>5278</v>
       </c>
       <c r="F32">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G32">
         <v>103.98278999999999</v>
@@ -1674,22 +1719,22 @@
         <v>40</v>
       </c>
       <c r="B33">
-        <v>11889</v>
+        <v>5391</v>
       </c>
       <c r="C33">
-        <v>36</v>
+        <v>6</v>
       </c>
       <c r="D33">
+        <v>96.322599999999994</v>
+      </c>
+      <c r="E33">
+        <v>4374</v>
+      </c>
+      <c r="F33">
+        <v>5</v>
+      </c>
+      <c r="G33">
         <v>96.486810000000006</v>
-      </c>
-      <c r="E33">
-        <v>12580</v>
-      </c>
-      <c r="F33">
-        <v>43</v>
-      </c>
-      <c r="G33">
-        <v>97.800529999999995</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
@@ -1697,22 +1742,22 @@
         <v>41</v>
       </c>
       <c r="B34">
-        <v>15257</v>
+        <v>7288</v>
       </c>
       <c r="C34">
-        <v>2877</v>
+        <v>11</v>
       </c>
       <c r="D34">
-        <v>101.69239</v>
+        <v>101.528175</v>
       </c>
       <c r="E34">
-        <v>14274</v>
+        <v>5708</v>
       </c>
       <c r="F34">
-        <v>70</v>
+        <v>8</v>
       </c>
       <c r="G34">
-        <v>101.69239</v>
+        <v>101.528175</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
@@ -1723,19 +1768,19 @@
         <v>15743</v>
       </c>
       <c r="C35">
-        <v>84</v>
+        <v>42</v>
       </c>
       <c r="D35">
         <v>183.05538999999999</v>
       </c>
       <c r="E35">
-        <v>15743</v>
+        <v>15644</v>
       </c>
       <c r="F35">
-        <v>73</v>
+        <v>45</v>
       </c>
       <c r="G35">
-        <v>185.02597</v>
+        <v>183.05538999999999</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
@@ -1743,22 +1788,22 @@
         <v>43</v>
       </c>
       <c r="B36">
-        <v>11888</v>
+        <v>5349</v>
       </c>
       <c r="C36">
-        <v>41</v>
+        <v>6</v>
       </c>
       <c r="D36">
+        <v>97.943923999999996</v>
+      </c>
+      <c r="E36">
+        <v>4281</v>
+      </c>
+      <c r="F36">
+        <v>5</v>
+      </c>
+      <c r="G36">
         <v>98.108130000000003</v>
-      </c>
-      <c r="E36">
-        <v>12579</v>
-      </c>
-      <c r="F36">
-        <v>33</v>
-      </c>
-      <c r="G36">
-        <v>98.764989999999997</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
@@ -1766,19 +1811,19 @@
         <v>44</v>
       </c>
       <c r="B37">
-        <v>12052</v>
+        <v>4737</v>
       </c>
       <c r="C37">
-        <v>24</v>
+        <v>5</v>
       </c>
       <c r="D37">
         <v>108.12008</v>
       </c>
       <c r="E37">
-        <v>14000</v>
+        <v>3721</v>
       </c>
       <c r="F37">
-        <v>32</v>
+        <v>4</v>
       </c>
       <c r="G37">
         <v>108.12008</v>
@@ -1789,22 +1834,22 @@
         <v>45</v>
       </c>
       <c r="B38">
-        <v>15703</v>
+        <v>15672</v>
       </c>
       <c r="C38">
-        <v>72</v>
+        <v>37</v>
       </c>
       <c r="D38">
         <v>164.22695999999999</v>
       </c>
       <c r="E38">
-        <v>15699</v>
+        <v>15420</v>
       </c>
       <c r="F38">
-        <v>72</v>
+        <v>2025</v>
       </c>
       <c r="G38">
-        <v>164.71960000000001</v>
+        <v>164.22695999999999</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
@@ -1812,19 +1857,19 @@
         <v>46</v>
       </c>
       <c r="B39">
-        <v>14629</v>
+        <v>7493</v>
       </c>
       <c r="C39">
-        <v>56</v>
+        <v>10</v>
       </c>
       <c r="D39">
         <v>92.363960000000006</v>
       </c>
       <c r="E39">
-        <v>14486</v>
+        <v>5491</v>
       </c>
       <c r="F39">
-        <v>3137</v>
+        <v>7</v>
       </c>
       <c r="G39">
         <v>92.363960000000006</v>
@@ -1835,22 +1880,22 @@
         <v>47</v>
       </c>
       <c r="B40">
-        <v>14877</v>
+        <v>8678</v>
       </c>
       <c r="C40">
-        <v>29</v>
+        <v>12</v>
       </c>
       <c r="D40">
         <v>109.57259999999999</v>
       </c>
       <c r="E40">
-        <v>14638</v>
+        <v>6124</v>
       </c>
       <c r="F40">
-        <v>29</v>
+        <v>8</v>
       </c>
       <c r="G40">
-        <v>110.80636</v>
+        <v>110.97057</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
@@ -1858,19 +1903,19 @@
         <v>48</v>
       </c>
       <c r="B41">
-        <v>5443</v>
+        <v>5246</v>
       </c>
       <c r="C41">
-        <v>8</v>
+        <v>73</v>
       </c>
       <c r="D41">
-        <v>95.363969999999995</v>
+        <v>95.199749999999995</v>
       </c>
       <c r="E41">
-        <v>4208</v>
+        <v>4122</v>
       </c>
       <c r="F41">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G41">
         <v>95.363969999999995</v>
@@ -1881,19 +1926,19 @@
         <v>49</v>
       </c>
       <c r="B42">
-        <v>15743</v>
+        <v>15520</v>
       </c>
       <c r="C42">
-        <v>88</v>
+        <v>31</v>
       </c>
       <c r="D42">
         <v>164.12897000000001</v>
       </c>
       <c r="E42">
-        <v>15733</v>
+        <v>13582</v>
       </c>
       <c r="F42">
-        <v>101</v>
+        <v>26</v>
       </c>
       <c r="G42">
         <v>164.12897000000001</v>
@@ -1904,22 +1949,22 @@
         <v>50</v>
       </c>
       <c r="B43">
-        <v>14795</v>
+        <v>11762</v>
       </c>
       <c r="C43">
-        <v>370</v>
+        <v>28</v>
       </c>
       <c r="D43">
         <v>117.98833500000001</v>
       </c>
       <c r="E43">
-        <v>14541</v>
+        <v>9978</v>
       </c>
       <c r="F43">
-        <v>52</v>
+        <v>23</v>
       </c>
       <c r="G43">
-        <v>118.23098</v>
+        <v>117.74569</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
@@ -1927,22 +1972,22 @@
         <v>51</v>
       </c>
       <c r="B44">
-        <v>11297</v>
+        <v>10884</v>
       </c>
       <c r="C44">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D44">
         <v>123.150406</v>
       </c>
       <c r="E44">
-        <v>8635</v>
+        <v>7935</v>
       </c>
       <c r="F44">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="G44">
-        <v>124.95677000000001</v>
+        <v>124.29991</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
@@ -1950,19 +1995,19 @@
         <v>52</v>
       </c>
       <c r="B45">
-        <v>15202</v>
+        <v>10558</v>
       </c>
       <c r="C45">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="D45">
         <v>116.18226</v>
       </c>
       <c r="E45">
-        <v>15163</v>
+        <v>7566</v>
       </c>
       <c r="F45">
-        <v>98</v>
+        <v>10</v>
       </c>
       <c r="G45">
         <v>116.18226</v>
@@ -1973,22 +2018,22 @@
         <v>53</v>
       </c>
       <c r="B46">
-        <v>13725</v>
+        <v>5213</v>
       </c>
       <c r="C46">
-        <v>35</v>
+        <v>7</v>
       </c>
       <c r="D46">
         <v>81.069810000000004</v>
       </c>
       <c r="E46">
-        <v>15390</v>
+        <v>3845</v>
       </c>
       <c r="F46">
-        <v>36</v>
+        <v>5</v>
       </c>
       <c r="G46">
-        <v>82.876170000000002</v>
+        <v>81.069810000000004</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
@@ -1996,19 +2041,19 @@
         <v>54</v>
       </c>
       <c r="B47">
-        <v>15635</v>
+        <v>11800</v>
       </c>
       <c r="C47">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="D47">
         <v>122.534294</v>
       </c>
       <c r="E47">
-        <v>15714</v>
+        <v>6882</v>
       </c>
       <c r="F47">
-        <v>67</v>
+        <v>9</v>
       </c>
       <c r="G47">
         <v>122.534294</v>
@@ -2019,19 +2064,19 @@
         <v>55</v>
       </c>
       <c r="B48">
-        <v>15735</v>
+        <v>14578</v>
       </c>
       <c r="C48">
-        <v>38</v>
+        <v>28</v>
       </c>
       <c r="D48">
         <v>137.98708999999999</v>
       </c>
       <c r="E48">
-        <v>15734</v>
+        <v>9979</v>
       </c>
       <c r="F48">
-        <v>43</v>
+        <v>19</v>
       </c>
       <c r="G48">
         <v>137.98708999999999</v>
@@ -2042,22 +2087,22 @@
         <v>56</v>
       </c>
       <c r="B49">
-        <v>15628</v>
+        <v>15329</v>
       </c>
       <c r="C49">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D49">
         <v>135.40129999999999</v>
       </c>
       <c r="E49">
-        <v>15630</v>
+        <v>14453</v>
       </c>
       <c r="F49">
-        <v>53</v>
+        <v>138</v>
       </c>
       <c r="G49">
-        <v>135.40129999999999</v>
+        <v>141.06244000000001</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
@@ -2065,22 +2110,22 @@
         <v>57</v>
       </c>
       <c r="B50">
-        <v>6228</v>
+        <v>2343</v>
       </c>
       <c r="C50">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="D50">
         <v>53.087310000000002</v>
       </c>
       <c r="E50">
-        <v>6493</v>
+        <v>1102</v>
       </c>
       <c r="F50">
-        <v>22</v>
+        <v>1</v>
       </c>
       <c r="G50">
-        <v>53.087310000000002</v>
+        <v>54.072600000000001</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
@@ -2088,22 +2133,22 @@
         <v>58</v>
       </c>
       <c r="B51">
-        <v>15652</v>
+        <v>12845</v>
       </c>
       <c r="C51">
-        <v>89</v>
+        <v>21</v>
       </c>
       <c r="D51">
         <v>114.32197600000001</v>
       </c>
       <c r="E51">
-        <v>15655</v>
+        <v>9480</v>
       </c>
       <c r="F51">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="G51">
-        <v>114.32197600000001</v>
+        <v>115.75702</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
@@ -2111,22 +2156,22 @@
         <v>59</v>
       </c>
       <c r="B52">
-        <v>9746</v>
+        <v>3810</v>
       </c>
       <c r="C52">
-        <v>21</v>
+        <v>5</v>
       </c>
       <c r="D52">
         <v>56.584519999999998</v>
       </c>
       <c r="E52">
-        <v>13734</v>
+        <v>2506</v>
       </c>
       <c r="F52">
-        <v>29</v>
+        <v>3</v>
       </c>
       <c r="G52">
-        <v>57.405594000000001</v>
+        <v>56.584519999999998</v>
       </c>
     </row>
   </sheetData>
@@ -2139,7 +2184,7 @@
   <dimension ref="A1:M52"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:M2"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>